<commit_message>
Updates after correction to Fiohog
</commit_message>
<xml_diff>
--- a/Figures/TestResults.xlsx
+++ b/Figures/TestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eoin/Work/PhdThesis/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0601AF30-151A-974A-9F33-C46117F8959B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB8A81E-EA4E-C243-BC2B-3088CF960D72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="720" windowWidth="27340" windowHeight="15580" activeTab="1" xr2:uid="{BDA54389-B7CA-EC41-A61F-DEAE829EE646}"/>
+    <workbookView xWindow="720" yWindow="2880" windowWidth="27340" windowHeight="14440" xr2:uid="{BDA54389-B7CA-EC41-A61F-DEAE829EE646}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="263">
   <si>
     <t>Scenario</t>
   </si>
@@ -967,6 +967,42 @@
   <si>
     <t>It uses considerably less CPU than the set in "pidstat - set 3" but it isn't clear why.</t>
   </si>
+  <si>
+    <t>The data tests below are probably invalid as I realised that the reusable data block creation was (accidentally) being done on each request (!)</t>
+  </si>
+  <si>
+    <t>datasize-tests-20180817</t>
+  </si>
+  <si>
+    <t>20180817-234956</t>
+  </si>
+  <si>
+    <t>20180817-234549</t>
+  </si>
+  <si>
+    <t>20180817-234632</t>
+  </si>
+  <si>
+    <t>20180817-234716</t>
+  </si>
+  <si>
+    <t>20180817-235054</t>
+  </si>
+  <si>
+    <t>20180817-235213</t>
+  </si>
+  <si>
+    <t>20180817-235331</t>
+  </si>
+  <si>
+    <t>20180817-234800</t>
+  </si>
+  <si>
+    <t>20180817-234858</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
 </sst>
 </file>
 
@@ -1045,7 +1081,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1094,6 +1130,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1108,7 +1150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1155,6 +1197,8 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7086,9 +7130,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$C$46:$C$57</c:f>
+              <c:f>Results!$C$46:$C$54</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>data-100mbx4</c:v>
                 </c:pt>
@@ -7099,30 +7143,21 @@
                   <c:v>data-100mbx4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>data-500mbx4</c:v>
+                  <c:v>data-1gbx4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>data-500mbx4</c:v>
+                  <c:v>data-1gbx4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>data-500mbx4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>data-1gbx4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>data-1gbx4</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>data-1gbx4</c:v>
                 </c:pt>
               </c:strCache>
@@ -7130,45 +7165,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$L$46:$L$57</c:f>
+              <c:f>Results!$L$46:$L$54</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1742</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>258</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>255</c:v>
+                  <c:v>3282</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>3648</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>242</c:v>
+                  <c:v>3523</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3904</c:v>
+                  <c:v>8541</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3496</c:v>
+                  <c:v>8265</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3445</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7585</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7269</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7396</c:v>
+                  <c:v>8820</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7228,9 +7254,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$C$46:$C$57</c:f>
+              <c:f>Results!$C$46:$C$54</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>data-100mbx4</c:v>
                 </c:pt>
@@ -7241,30 +7267,21 @@
                   <c:v>data-100mbx4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>data-500mbx4</c:v>
+                  <c:v>data-1gbx4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>data-500mbx4</c:v>
+                  <c:v>data-1gbx4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>data-500mbx4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>data-1gbx4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>data-1gbx4</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>data-1gbx4</c:v>
                 </c:pt>
               </c:strCache>
@@ -7272,45 +7289,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$Q$46:$Q$57</c:f>
+              <c:f>Results!$Q$46:$Q$54</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>293</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>328</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>339</c:v>
+                  <c:v>707</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>303</c:v>
+                  <c:v>671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>661</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>644</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>621</c:v>
+                  <c:v>721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7837,9 +7845,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$C$47:$C$57</c:f>
+              <c:f>Results!$C$47:$C$54</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>data-100mbx4</c:v>
                 </c:pt>
@@ -7847,30 +7855,21 @@
                   <c:v>data-100mbx4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>data-500mbx4</c:v>
+                  <c:v>data-1gbx4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>data-500mbx4</c:v>
+                  <c:v>data-1gbx4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>data-500mbx4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>data-1gbx4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>data-1gbx4</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>data-1gbx4</c:v>
                 </c:pt>
               </c:strCache>
@@ -7878,10 +7877,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$K$47:$K$57</c:f>
+              <c:f>Results!$K$47:$K$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>400</c:v>
                 </c:pt>
@@ -7889,30 +7888,21 @@
                   <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>400</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2000</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2000</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>4000</c:v>
                 </c:pt>
               </c:numCache>
@@ -7973,9 +7963,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$C$47:$C$57</c:f>
+              <c:f>Results!$C$47:$C$54</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>data-100mbx4</c:v>
                 </c:pt>
@@ -7983,30 +7973,21 @@
                   <c:v>data-100mbx4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>data-100mbx4</c:v>
+                  <c:v>data-500mbx4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>data-500mbx4</c:v>
+                  <c:v>data-1gbx4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>data-500mbx4</c:v>
+                  <c:v>data-1gbx4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>data-500mbx4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>data-1gbx4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>data-1gbx4</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>data-1gbx4</c:v>
                 </c:pt>
               </c:strCache>
@@ -8014,42 +7995,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$O$47:$O$57</c:f>
+              <c:f>Results!$O$47:$O$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44</c:v>
+                  <c:v>328</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>339</c:v>
+                  <c:v>707</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>303</c:v>
+                  <c:v>671</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>661</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>644</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>621</c:v>
+                  <c:v>721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8564,7 +8536,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$C$58:$C$69</c:f>
+              <c:f>Results!$C$55:$C$66</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -8608,7 +8580,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$L$58:$L$69</c:f>
+              <c:f>Results!$L$55:$L$66</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
@@ -8694,7 +8666,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Results!$C$58:$C$69</c:f>
+              <c:f>Results!$C$55:$C$66</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -8738,7 +8710,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results!$Q$58:$Q$69</c:f>
+              <c:f>Results!$Q$55:$Q$66</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
@@ -14646,16 +14618,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A7A84C-38BB-9C46-BB61-734C431F3DDA}">
-  <dimension ref="B2:S90"/>
+  <dimension ref="A2:S96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
@@ -14760,7 +14732,7 @@
         <v>226900</v>
       </c>
       <c r="L5" s="10">
-        <f t="shared" ref="L5:L57" si="0">I5/D5</f>
+        <f t="shared" ref="L5:L45" si="0">I5/D5</f>
         <v>22690</v>
       </c>
       <c r="M5" s="9">
@@ -14777,7 +14749,7 @@
         <v>0.10027324812692816</v>
       </c>
       <c r="Q5" s="10">
-        <f t="shared" ref="Q5:Q57" si="1">O5/D5</f>
+        <f t="shared" ref="Q5:Q45" si="1">O5/D5</f>
         <v>2275.1999999999998</v>
       </c>
       <c r="R5" s="9">
@@ -16252,7 +16224,7 @@
         <v>13529</v>
       </c>
       <c r="P34" s="7">
-        <f t="shared" ref="P34:P57" si="5">O34/I34</f>
+        <f t="shared" ref="P34:P45" si="5">O34/I34</f>
         <v>0.10725214440868228</v>
       </c>
       <c r="Q34" s="8">
@@ -16277,7 +16249,7 @@
         <v>70</v>
       </c>
       <c r="F35" s="9" t="str">
-        <f t="shared" ref="F35:F57" si="6">LEFT(E35, 8)</f>
+        <f t="shared" ref="F35:F54" si="6">LEFT(E35, 8)</f>
         <v>20180808</v>
       </c>
       <c r="G35" s="7">
@@ -16826,7 +16798,7 @@
     </row>
     <row r="46" spans="2:18" s="23" customFormat="1">
       <c r="B46" s="23" t="s">
-        <v>124</v>
+        <v>252</v>
       </c>
       <c r="C46" s="23" t="s">
         <v>125</v>
@@ -16835,20 +16807,20 @@
         <v>1</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>126</v>
+        <v>254</v>
       </c>
       <c r="F46" s="23" t="str">
         <f>LEFT(E46, 8)</f>
-        <v>20180813</v>
+        <v>20180817</v>
       </c>
       <c r="G46" s="23">
         <v>0</v>
       </c>
       <c r="H46" s="23">
-        <v>3135</v>
+        <v>2561</v>
       </c>
       <c r="I46" s="23">
-        <v>1742</v>
+        <v>188</v>
       </c>
       <c r="J46" s="23">
         <v>400</v>
@@ -16859,32 +16831,32 @@
       </c>
       <c r="L46" s="24">
         <f>I46/D46</f>
-        <v>1742</v>
+        <v>188</v>
       </c>
       <c r="M46" s="23">
-        <v>1605</v>
+        <v>556</v>
       </c>
       <c r="N46" s="23">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="O46" s="23">
-        <v>293</v>
+        <v>44</v>
       </c>
       <c r="P46" s="23">
         <f>O46/I46</f>
-        <v>0.16819747416762343</v>
+        <v>0.23404255319148937</v>
       </c>
       <c r="Q46" s="24">
         <f>O46/D46</f>
-        <v>293</v>
+        <v>44</v>
       </c>
       <c r="R46" s="23">
-        <v>270</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="2:18" s="23" customFormat="1">
       <c r="B47" s="23" t="s">
-        <v>124</v>
+        <v>252</v>
       </c>
       <c r="C47" s="23" t="s">
         <v>125</v>
@@ -16893,56 +16865,56 @@
         <v>1</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="F47" s="23" t="str">
         <f>LEFT(E47, 8)</f>
-        <v>20180813</v>
+        <v>20180817</v>
       </c>
       <c r="G47" s="23">
         <v>0</v>
       </c>
       <c r="H47" s="23">
-        <v>2565</v>
+        <v>2556</v>
       </c>
       <c r="I47" s="23">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="J47" s="23">
         <v>400</v>
       </c>
       <c r="K47" s="23">
-        <f t="shared" ref="K47:K69" si="7">J47/D47</f>
+        <f>J47/D47</f>
         <v>400</v>
       </c>
       <c r="L47" s="24">
         <f>I47/D47</f>
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="M47" s="23">
-        <v>972</v>
+        <v>1066</v>
       </c>
       <c r="N47" s="23">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O47" s="23">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P47" s="23">
         <f>O47/I47</f>
-        <v>0.17054263565891473</v>
+        <v>0.16304347826086957</v>
       </c>
       <c r="Q47" s="24">
         <f>O47/D47</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R47" s="23">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="2:18" s="23" customFormat="1">
       <c r="B48" s="23" t="s">
-        <v>124</v>
+        <v>252</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>125</v>
@@ -16951,11 +16923,11 @@
         <v>1</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="F48" s="23" t="str">
         <f>LEFT(E48, 8)</f>
-        <v>20180813</v>
+        <v>20180817</v>
       </c>
       <c r="G48" s="23">
         <v>0</v>
@@ -16964,574 +16936,586 @@
         <v>2567</v>
       </c>
       <c r="I48" s="23">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="J48" s="23">
         <v>400</v>
       </c>
       <c r="K48" s="23">
-        <f t="shared" si="7"/>
+        <f>J48/D48</f>
         <v>400</v>
       </c>
       <c r="L48" s="24">
         <f>I48/D48</f>
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="M48" s="23">
-        <v>976</v>
+        <v>955</v>
       </c>
       <c r="N48" s="23">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O48" s="23">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P48" s="23">
         <f>O48/I48</f>
-        <v>0.17602996254681649</v>
+        <v>0.17204301075268819</v>
       </c>
       <c r="Q48" s="24">
         <f>O48/D48</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R48" s="23">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="49" spans="2:18" s="23" customFormat="1">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" s="23" customFormat="1">
       <c r="B49" s="23" t="s">
-        <v>137</v>
+        <v>252</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D49" s="23">
         <v>1</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>138</v>
+        <v>260</v>
       </c>
       <c r="F49" s="23" t="str">
         <f>LEFT(E49, 8)</f>
-        <v>20180814</v>
+        <v>20180817</v>
       </c>
       <c r="G49" s="23">
         <v>0</v>
       </c>
       <c r="H49" s="23">
-        <v>2551</v>
+        <v>16539</v>
       </c>
       <c r="I49" s="23">
-        <v>255</v>
+        <v>3282</v>
       </c>
       <c r="J49" s="23">
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="K49" s="23">
-        <f t="shared" si="7"/>
-        <v>400</v>
+        <f>J49/D49</f>
+        <v>2000</v>
       </c>
       <c r="L49" s="24">
         <f>I49/D49</f>
-        <v>255</v>
+        <v>3282</v>
       </c>
       <c r="M49" s="23">
-        <v>954</v>
+        <v>24249</v>
       </c>
       <c r="N49" s="23">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="O49" s="23">
-        <v>43</v>
+        <v>285</v>
       </c>
       <c r="P49" s="23">
         <f>O49/I49</f>
-        <v>0.16862745098039217</v>
+        <v>8.6837294332723955E-2</v>
       </c>
       <c r="Q49" s="24">
         <f>O49/D49</f>
-        <v>43</v>
+        <v>285</v>
       </c>
       <c r="R49" s="23">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="2:18" s="23" customFormat="1">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" s="23" customFormat="1">
       <c r="B50" s="23" t="s">
-        <v>137</v>
+        <v>252</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D50" s="23">
         <v>1</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>139</v>
+        <v>261</v>
       </c>
       <c r="F50" s="23" t="str">
         <f>LEFT(E50, 8)</f>
-        <v>20180814</v>
+        <v>20180817</v>
       </c>
       <c r="G50" s="23">
         <v>0</v>
       </c>
       <c r="H50" s="23">
-        <v>2558</v>
+        <v>16558</v>
       </c>
       <c r="I50" s="23">
-        <v>150</v>
+        <v>3648</v>
       </c>
       <c r="J50" s="23">
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="K50" s="23">
-        <f t="shared" si="7"/>
-        <v>400</v>
+        <f>J50/D50</f>
+        <v>2000</v>
       </c>
       <c r="L50" s="24">
         <f>I50/D50</f>
-        <v>150</v>
+        <v>3648</v>
       </c>
       <c r="M50" s="23">
-        <v>1018</v>
+        <v>23331</v>
       </c>
       <c r="N50" s="23">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O50" s="23">
-        <v>26</v>
+        <v>320</v>
       </c>
       <c r="P50" s="23">
         <f>O50/I50</f>
-        <v>0.17333333333333334</v>
+        <v>8.771929824561403E-2</v>
       </c>
       <c r="Q50" s="24">
         <f>O50/D50</f>
-        <v>26</v>
+        <v>320</v>
       </c>
       <c r="R50" s="23">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" spans="2:18" s="23" customFormat="1">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" s="23" customFormat="1">
       <c r="B51" s="23" t="s">
-        <v>137</v>
+        <v>252</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D51" s="23">
         <v>1</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>140</v>
+        <v>253</v>
       </c>
       <c r="F51" s="23" t="str">
         <f>LEFT(E51, 8)</f>
-        <v>20180814</v>
+        <v>20180817</v>
       </c>
       <c r="G51" s="23">
         <v>0</v>
       </c>
       <c r="H51" s="23">
-        <v>2560</v>
+        <v>16611</v>
       </c>
       <c r="I51" s="23">
-        <v>242</v>
+        <v>3523</v>
       </c>
       <c r="J51" s="23">
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="K51" s="23">
-        <f t="shared" si="7"/>
-        <v>400</v>
+        <f>J51/D51</f>
+        <v>2000</v>
       </c>
       <c r="L51" s="24">
         <f>I51/D51</f>
-        <v>242</v>
+        <v>3523</v>
       </c>
       <c r="M51" s="23">
-        <v>893</v>
+        <v>21221</v>
       </c>
       <c r="N51" s="23">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="O51" s="23">
-        <v>44</v>
+        <v>328</v>
       </c>
       <c r="P51" s="23">
         <f>O51/I51</f>
-        <v>0.18181818181818182</v>
+        <v>9.3102469486233325E-2</v>
       </c>
       <c r="Q51" s="24">
         <f>O51/D51</f>
-        <v>44</v>
+        <v>328</v>
       </c>
       <c r="R51" s="23">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="2:18" s="23" customFormat="1">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" s="23" customFormat="1">
       <c r="B52" s="23" t="s">
-        <v>124</v>
+        <v>252</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D52" s="23">
         <v>1</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>134</v>
+        <v>257</v>
       </c>
       <c r="F52" s="23" t="str">
         <f>LEFT(E52, 8)</f>
-        <v>20180813</v>
+        <v>20180817</v>
       </c>
       <c r="G52" s="23">
         <v>0</v>
       </c>
       <c r="H52" s="23">
-        <v>16498</v>
+        <v>36769</v>
       </c>
       <c r="I52" s="23">
-        <v>3904</v>
+        <v>8541</v>
       </c>
       <c r="J52" s="23">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="K52" s="23">
-        <f t="shared" si="7"/>
-        <v>2000</v>
+        <f>J52/D52</f>
+        <v>4000</v>
       </c>
       <c r="L52" s="24">
         <f>I52/D52</f>
-        <v>3904</v>
+        <v>8541</v>
       </c>
       <c r="M52" s="23">
-        <v>23889</v>
+        <v>59822</v>
       </c>
       <c r="N52" s="23">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O52" s="23">
-        <v>339</v>
+        <v>707</v>
       </c>
       <c r="P52" s="23">
         <f>O52/I52</f>
-        <v>8.6834016393442626E-2</v>
+        <v>8.277719236623346E-2</v>
       </c>
       <c r="Q52" s="24">
         <f>O52/D52</f>
-        <v>339</v>
+        <v>707</v>
       </c>
       <c r="R52" s="23">
-        <v>2074</v>
-      </c>
-    </row>
-    <row r="53" spans="2:18" s="23" customFormat="1">
+        <v>4946</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" s="23" customFormat="1">
       <c r="B53" s="23" t="s">
-        <v>124</v>
+        <v>252</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D53" s="23">
         <v>1</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>135</v>
+        <v>258</v>
       </c>
       <c r="F53" s="23" t="str">
         <f>LEFT(E53, 8)</f>
-        <v>20180813</v>
+        <v>20180817</v>
       </c>
       <c r="G53" s="23">
         <v>0</v>
       </c>
       <c r="H53" s="23">
-        <v>16518</v>
+        <v>36896</v>
       </c>
       <c r="I53" s="23">
-        <v>3496</v>
+        <v>8265</v>
       </c>
       <c r="J53" s="23">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="K53" s="23">
-        <f t="shared" si="7"/>
-        <v>2000</v>
+        <f>J53/D53</f>
+        <v>4000</v>
       </c>
       <c r="L53" s="24">
         <f>I53/D53</f>
-        <v>3496</v>
+        <v>8265</v>
       </c>
       <c r="M53" s="23">
-        <v>24308</v>
+        <v>60896</v>
       </c>
       <c r="N53" s="23">
         <v>14</v>
       </c>
       <c r="O53" s="23">
-        <v>303</v>
+        <v>671</v>
       </c>
       <c r="P53" s="23">
         <f>O53/I53</f>
-        <v>8.6670480549199083E-2</v>
+        <v>8.1185722928009685E-2</v>
       </c>
       <c r="Q53" s="24">
         <f>O53/D53</f>
-        <v>303</v>
+        <v>671</v>
       </c>
       <c r="R53" s="23">
-        <v>2099</v>
-      </c>
-    </row>
-    <row r="54" spans="2:18" s="23" customFormat="1">
+        <v>4946</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" s="23" customFormat="1">
       <c r="B54" s="23" t="s">
-        <v>124</v>
+        <v>252</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D54" s="23">
         <v>1</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>136</v>
+        <v>259</v>
       </c>
       <c r="F54" s="23" t="str">
         <f>LEFT(E54, 8)</f>
-        <v>20180813</v>
+        <v>20180817</v>
       </c>
       <c r="G54" s="23">
         <v>0</v>
       </c>
       <c r="H54" s="23">
-        <v>17272</v>
+        <v>36892</v>
       </c>
       <c r="I54" s="23">
-        <v>3445</v>
+        <v>8820</v>
       </c>
       <c r="J54" s="23">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="K54" s="23">
-        <f t="shared" si="7"/>
-        <v>2000</v>
+        <f>J54/D54</f>
+        <v>4000</v>
       </c>
       <c r="L54" s="24">
         <f>I54/D54</f>
-        <v>3445</v>
+        <v>8820</v>
       </c>
       <c r="M54" s="23">
-        <v>35363</v>
+        <v>60502</v>
       </c>
       <c r="N54" s="23">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="O54" s="23">
-        <v>250</v>
+        <v>721</v>
       </c>
       <c r="P54" s="23">
         <f>O54/I54</f>
-        <v>7.2568940493468792E-2</v>
+        <v>8.1746031746031747E-2</v>
       </c>
       <c r="Q54" s="24">
         <f>O54/D54</f>
-        <v>250</v>
+        <v>721</v>
       </c>
       <c r="R54" s="23">
-        <v>2572</v>
-      </c>
-    </row>
-    <row r="55" spans="2:18" s="23" customFormat="1">
-      <c r="B55" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="C55" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="D55" s="23">
-        <v>1</v>
-      </c>
-      <c r="E55" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="F55" s="23" t="str">
+        <v>4946</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" s="25" customFormat="1">
+      <c r="A55" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="25">
+        <v>5</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="F55" s="25" t="str">
         <f>LEFT(E55, 8)</f>
-        <v>20180813</v>
-      </c>
-      <c r="G55" s="23">
-        <v>0</v>
-      </c>
-      <c r="H55" s="23">
-        <v>36711</v>
-      </c>
-      <c r="I55" s="23">
-        <v>7585</v>
-      </c>
-      <c r="J55" s="23">
-        <v>4000</v>
-      </c>
-      <c r="K55" s="23">
+        <v>20180814</v>
+      </c>
+      <c r="G55" s="25">
+        <v>0</v>
+      </c>
+      <c r="H55" s="25">
+        <v>23893</v>
+      </c>
+      <c r="I55" s="25">
+        <v>5864</v>
+      </c>
+      <c r="J55" s="25">
+        <v>3000</v>
+      </c>
+      <c r="K55" s="25">
+        <f t="shared" ref="K47:K66" si="7">J55/D55</f>
+        <v>600</v>
+      </c>
+      <c r="L55" s="26">
+        <f>I55/D55</f>
+        <v>1172.8</v>
+      </c>
+      <c r="M55" s="25">
+        <v>29547</v>
+      </c>
+      <c r="N55" s="25">
+        <v>20</v>
+      </c>
+      <c r="O55" s="25">
+        <v>555</v>
+      </c>
+      <c r="P55" s="25">
+        <f>O55/I55</f>
+        <v>9.464529331514325E-2</v>
+      </c>
+      <c r="Q55" s="26">
+        <f>O55/D55</f>
+        <v>111</v>
+      </c>
+      <c r="R55" s="25">
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" s="25" customFormat="1">
+      <c r="A56" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" s="25">
+        <v>5</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F56" s="25" t="str">
+        <f>LEFT(E56, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G56" s="25">
+        <v>0</v>
+      </c>
+      <c r="H56" s="25">
+        <v>24253</v>
+      </c>
+      <c r="I56" s="25">
+        <v>6137</v>
+      </c>
+      <c r="J56" s="25">
+        <v>3000</v>
+      </c>
+      <c r="K56" s="25">
         <f t="shared" si="7"/>
-        <v>4000</v>
-      </c>
-      <c r="L55" s="24">
-        <f>I55/D55</f>
-        <v>7585</v>
-      </c>
-      <c r="M55" s="23">
-        <v>53502</v>
-      </c>
-      <c r="N55" s="23">
-        <v>14</v>
-      </c>
-      <c r="O55" s="23">
-        <v>661</v>
-      </c>
-      <c r="P55" s="23">
-        <f>O55/I55</f>
-        <v>8.7145682267633487E-2</v>
-      </c>
-      <c r="Q55" s="24">
-        <f>O55/D55</f>
-        <v>661</v>
-      </c>
-      <c r="R55" s="23">
-        <v>4666</v>
-      </c>
-    </row>
-    <row r="56" spans="2:18" s="23" customFormat="1">
-      <c r="B56" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="C56" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="D56" s="23">
-        <v>1</v>
-      </c>
-      <c r="E56" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="F56" s="23" t="str">
-        <f>LEFT(E56, 8)</f>
-        <v>20180813</v>
-      </c>
-      <c r="G56" s="23">
-        <v>0</v>
-      </c>
-      <c r="H56" s="23">
-        <v>36717</v>
-      </c>
-      <c r="I56" s="23">
-        <v>7269</v>
-      </c>
-      <c r="J56" s="23">
-        <v>4000</v>
-      </c>
-      <c r="K56" s="23">
+        <v>600</v>
+      </c>
+      <c r="L56" s="26">
+        <f>I56/D56</f>
+        <v>1227.4000000000001</v>
+      </c>
+      <c r="M56" s="25">
+        <v>33525</v>
+      </c>
+      <c r="N56" s="25">
+        <v>18</v>
+      </c>
+      <c r="O56" s="25">
+        <v>562</v>
+      </c>
+      <c r="P56" s="25">
+        <f>O56/I56</f>
+        <v>9.1575688447124007E-2</v>
+      </c>
+      <c r="Q56" s="26">
+        <f>O56/D56</f>
+        <v>112.4</v>
+      </c>
+      <c r="R56" s="25">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" s="25" customFormat="1">
+      <c r="A57" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D57" s="25">
+        <v>5</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F57" s="25" t="str">
+        <f>LEFT(E57, 8)</f>
+        <v>20180815</v>
+      </c>
+      <c r="G57" s="25">
+        <v>0</v>
+      </c>
+      <c r="H57" s="25">
+        <v>24959</v>
+      </c>
+      <c r="I57" s="25">
+        <v>9892</v>
+      </c>
+      <c r="J57" s="25">
+        <v>3000</v>
+      </c>
+      <c r="K57" s="25">
         <f t="shared" si="7"/>
-        <v>4000</v>
-      </c>
-      <c r="L56" s="24">
-        <f>I56/D56</f>
-        <v>7269</v>
-      </c>
-      <c r="M56" s="23">
-        <v>52664</v>
-      </c>
-      <c r="N56" s="23">
-        <v>14</v>
-      </c>
-      <c r="O56" s="23">
-        <v>644</v>
-      </c>
-      <c r="P56" s="23">
-        <f>O56/I56</f>
-        <v>8.8595405145136877E-2</v>
-      </c>
-      <c r="Q56" s="24">
-        <f>O56/D56</f>
-        <v>644</v>
-      </c>
-      <c r="R56" s="23">
-        <v>4666</v>
-      </c>
-    </row>
-    <row r="57" spans="2:18" s="23" customFormat="1">
-      <c r="B57" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="D57" s="23">
-        <v>1</v>
-      </c>
-      <c r="E57" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="F57" s="23" t="str">
-        <f>LEFT(E57, 8)</f>
-        <v>20180814</v>
-      </c>
-      <c r="G57" s="23">
-        <v>0</v>
-      </c>
-      <c r="H57" s="23">
-        <v>36829</v>
-      </c>
-      <c r="I57" s="23">
-        <v>7396</v>
-      </c>
-      <c r="J57" s="23">
-        <v>4000</v>
-      </c>
-      <c r="K57" s="23">
-        <f t="shared" si="7"/>
-        <v>4000</v>
-      </c>
-      <c r="L57" s="24">
+        <v>600</v>
+      </c>
+      <c r="L57" s="26">
         <f>I57/D57</f>
-        <v>7396</v>
-      </c>
-      <c r="M57" s="23">
-        <v>58227</v>
-      </c>
-      <c r="N57" s="23">
-        <v>13</v>
-      </c>
-      <c r="O57" s="23">
-        <v>621</v>
-      </c>
-      <c r="P57" s="23">
+        <v>1978.4</v>
+      </c>
+      <c r="M57" s="25">
+        <v>34604</v>
+      </c>
+      <c r="N57" s="25">
+        <v>29</v>
+      </c>
+      <c r="O57" s="25">
+        <v>879</v>
+      </c>
+      <c r="P57" s="25">
         <f>O57/I57</f>
-        <v>8.3964305029745806E-2</v>
-      </c>
-      <c r="Q57" s="24">
+        <v>8.8859684593611002E-2</v>
+      </c>
+      <c r="Q57" s="26">
         <f>O57/D57</f>
-        <v>621</v>
-      </c>
-      <c r="R57" s="23">
-        <v>4896</v>
-      </c>
-    </row>
-    <row r="58" spans="2:18" s="25" customFormat="1">
+        <v>175.8</v>
+      </c>
+      <c r="R57" s="25">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" s="25" customFormat="1">
+      <c r="A58" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="B58" s="25" t="s">
         <v>144</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D58" s="25">
         <v>5</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F58" s="25" t="str">
         <f>LEFT(E58, 8)</f>
@@ -17541,10 +17525,10 @@
         <v>0</v>
       </c>
       <c r="H58" s="25">
-        <v>23893</v>
+        <v>24316</v>
       </c>
       <c r="I58" s="25">
-        <v>5864</v>
+        <v>5809</v>
       </c>
       <c r="J58" s="25">
         <v>3000</v>
@@ -17555,41 +17539,44 @@
       </c>
       <c r="L58" s="26">
         <f>I58/D58</f>
-        <v>1172.8</v>
+        <v>1161.8</v>
       </c>
       <c r="M58" s="25">
-        <v>29547</v>
+        <v>31070</v>
       </c>
       <c r="N58" s="25">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O58" s="25">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="P58" s="25">
         <f>O58/I58</f>
-        <v>9.464529331514325E-2</v>
+        <v>9.5024961266999483E-2</v>
       </c>
       <c r="Q58" s="26">
         <f>O58/D58</f>
-        <v>111</v>
+        <v>110.4</v>
       </c>
       <c r="R58" s="25">
-        <v>2797</v>
-      </c>
-    </row>
-    <row r="59" spans="2:18" s="25" customFormat="1">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" s="25" customFormat="1">
+      <c r="A59" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="B59" s="25" t="s">
         <v>144</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D59" s="25">
         <v>5</v>
       </c>
       <c r="E59" s="25" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F59" s="25" t="str">
         <f>LEFT(E59, 8)</f>
@@ -17599,10 +17586,10 @@
         <v>0</v>
       </c>
       <c r="H59" s="25">
-        <v>24253</v>
+        <v>24557</v>
       </c>
       <c r="I59" s="25">
-        <v>6137</v>
+        <v>5725</v>
       </c>
       <c r="J59" s="25">
         <v>3000</v>
@@ -17613,41 +17600,44 @@
       </c>
       <c r="L59" s="26">
         <f>I59/D59</f>
-        <v>1227.4000000000001</v>
+        <v>1145</v>
       </c>
       <c r="M59" s="25">
-        <v>33525</v>
+        <v>32726</v>
       </c>
       <c r="N59" s="25">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O59" s="25">
-        <v>562</v>
+        <v>524</v>
       </c>
       <c r="P59" s="25">
         <f>O59/I59</f>
-        <v>9.1575688447124007E-2</v>
+        <v>9.1528384279475988E-2</v>
       </c>
       <c r="Q59" s="26">
         <f>O59/D59</f>
-        <v>112.4</v>
+        <v>104.8</v>
       </c>
       <c r="R59" s="25">
-        <v>3072</v>
-      </c>
-    </row>
-    <row r="60" spans="2:18" s="25" customFormat="1">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" s="25" customFormat="1">
+      <c r="A60" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="B60" s="25" t="s">
         <v>144</v>
       </c>
       <c r="C60" s="25" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D60" s="25">
         <v>5</v>
       </c>
       <c r="E60" s="25" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F60" s="25" t="str">
         <f>LEFT(E60, 8)</f>
@@ -17657,10 +17647,10 @@
         <v>0</v>
       </c>
       <c r="H60" s="25">
-        <v>24959</v>
+        <v>24133</v>
       </c>
       <c r="I60" s="25">
-        <v>9892</v>
+        <v>5796</v>
       </c>
       <c r="J60" s="25">
         <v>3000</v>
@@ -17671,41 +17661,44 @@
       </c>
       <c r="L60" s="26">
         <f>I60/D60</f>
-        <v>1978.4</v>
+        <v>1159.2</v>
       </c>
       <c r="M60" s="25">
-        <v>34604</v>
+        <v>33081</v>
       </c>
       <c r="N60" s="25">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="O60" s="25">
-        <v>879</v>
+        <v>532</v>
       </c>
       <c r="P60" s="25">
         <f>O60/I60</f>
-        <v>8.8859684593611002E-2</v>
+        <v>9.1787439613526575E-2</v>
       </c>
       <c r="Q60" s="26">
         <f>O60/D60</f>
-        <v>175.8</v>
+        <v>106.4</v>
       </c>
       <c r="R60" s="25">
-        <v>3072</v>
-      </c>
-    </row>
-    <row r="61" spans="2:18" s="25" customFormat="1">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" s="25" customFormat="1">
+      <c r="A61" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="B61" s="25" t="s">
         <v>144</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D61" s="25">
         <v>5</v>
       </c>
       <c r="E61" s="25" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F61" s="25" t="str">
         <f>LEFT(E61, 8)</f>
@@ -17715,10 +17708,10 @@
         <v>0</v>
       </c>
       <c r="H61" s="25">
-        <v>24316</v>
+        <v>24475</v>
       </c>
       <c r="I61" s="25">
-        <v>5809</v>
+        <v>5548</v>
       </c>
       <c r="J61" s="25">
         <v>3000</v>
@@ -17729,41 +17722,44 @@
       </c>
       <c r="L61" s="26">
         <f>I61/D61</f>
-        <v>1161.8</v>
+        <v>1109.5999999999999</v>
       </c>
       <c r="M61" s="25">
-        <v>31070</v>
+        <v>36414</v>
       </c>
       <c r="N61" s="25">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O61" s="25">
-        <v>552</v>
+        <v>479</v>
       </c>
       <c r="P61" s="25">
         <f>O61/I61</f>
-        <v>9.5024961266999483E-2</v>
+        <v>8.6337418889689974E-2</v>
       </c>
       <c r="Q61" s="26">
         <f>O61/D61</f>
-        <v>110.4</v>
+        <v>95.8</v>
       </c>
       <c r="R61" s="25">
-        <v>2957</v>
-      </c>
-    </row>
-    <row r="62" spans="2:18" s="25" customFormat="1">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" s="25" customFormat="1">
+      <c r="A62" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="B62" s="25" t="s">
         <v>144</v>
       </c>
       <c r="C62" s="25" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D62" s="25">
         <v>5</v>
       </c>
       <c r="E62" s="25" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F62" s="25" t="str">
         <f>LEFT(E62, 8)</f>
@@ -17773,10 +17769,10 @@
         <v>0</v>
       </c>
       <c r="H62" s="25">
-        <v>24557</v>
+        <v>24526</v>
       </c>
       <c r="I62" s="25">
-        <v>5725</v>
+        <v>5674</v>
       </c>
       <c r="J62" s="25">
         <v>3000</v>
@@ -17787,41 +17783,44 @@
       </c>
       <c r="L62" s="26">
         <f>I62/D62</f>
-        <v>1145</v>
+        <v>1134.8</v>
       </c>
       <c r="M62" s="25">
-        <v>32726</v>
+        <v>35180</v>
       </c>
       <c r="N62" s="25">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O62" s="25">
-        <v>524</v>
+        <v>502</v>
       </c>
       <c r="P62" s="25">
         <f>O62/I62</f>
-        <v>9.1528384279475988E-2</v>
+        <v>8.8473739866055695E-2</v>
       </c>
       <c r="Q62" s="26">
         <f>O62/D62</f>
-        <v>104.8</v>
+        <v>100.4</v>
       </c>
       <c r="R62" s="25">
-        <v>2995</v>
-      </c>
-    </row>
-    <row r="63" spans="2:18" s="25" customFormat="1">
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" s="25" customFormat="1">
+      <c r="A63" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="B63" s="25" t="s">
         <v>144</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D63" s="25">
         <v>5</v>
       </c>
       <c r="E63" s="25" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F63" s="25" t="str">
         <f>LEFT(E63, 8)</f>
@@ -17831,10 +17830,10 @@
         <v>0</v>
       </c>
       <c r="H63" s="25">
-        <v>24133</v>
+        <v>24729</v>
       </c>
       <c r="I63" s="25">
-        <v>5796</v>
+        <v>6905</v>
       </c>
       <c r="J63" s="25">
         <v>3000</v>
@@ -17845,41 +17844,44 @@
       </c>
       <c r="L63" s="26">
         <f>I63/D63</f>
-        <v>1159.2</v>
+        <v>1381</v>
       </c>
       <c r="M63" s="25">
-        <v>33081</v>
+        <v>36416</v>
       </c>
       <c r="N63" s="25">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O63" s="25">
-        <v>532</v>
+        <v>597</v>
       </c>
       <c r="P63" s="25">
         <f>O63/I63</f>
-        <v>9.1787439613526575E-2</v>
+        <v>8.6459087617668351E-2</v>
       </c>
       <c r="Q63" s="26">
         <f>O63/D63</f>
-        <v>106.4</v>
+        <v>119.4</v>
       </c>
       <c r="R63" s="25">
-        <v>3034</v>
-      </c>
-    </row>
-    <row r="64" spans="2:18" s="25" customFormat="1">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" s="25" customFormat="1">
+      <c r="A64" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="B64" s="25" t="s">
         <v>144</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D64" s="25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E64" s="25" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F64" s="25" t="str">
         <f>LEFT(E64, 8)</f>
@@ -17889,55 +17891,58 @@
         <v>0</v>
       </c>
       <c r="H64" s="25">
-        <v>24475</v>
+        <v>24831</v>
       </c>
       <c r="I64" s="25">
-        <v>5548</v>
+        <v>5888</v>
       </c>
       <c r="J64" s="25">
         <v>3000</v>
       </c>
       <c r="K64" s="25">
         <f t="shared" si="7"/>
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="L64" s="26">
         <f>I64/D64</f>
-        <v>1109.5999999999999</v>
+        <v>1962.6666666666667</v>
       </c>
       <c r="M64" s="25">
-        <v>36414</v>
+        <v>37327</v>
       </c>
       <c r="N64" s="25">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O64" s="25">
-        <v>479</v>
+        <v>503</v>
       </c>
       <c r="P64" s="25">
         <f>O64/I64</f>
-        <v>8.6337418889689974E-2</v>
+        <v>8.5427989130434784E-2</v>
       </c>
       <c r="Q64" s="26">
         <f>O64/D64</f>
-        <v>95.8</v>
+        <v>167.66666666666666</v>
       </c>
       <c r="R64" s="25">
-        <v>3149</v>
-      </c>
-    </row>
-    <row r="65" spans="2:18" s="25" customFormat="1">
+        <v>3187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" s="25" customFormat="1">
+      <c r="A65" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="B65" s="25" t="s">
         <v>144</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D65" s="25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E65" s="25" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F65" s="25" t="str">
         <f>LEFT(E65, 8)</f>
@@ -17947,55 +17952,58 @@
         <v>0</v>
       </c>
       <c r="H65" s="25">
-        <v>24526</v>
+        <v>24891</v>
       </c>
       <c r="I65" s="25">
-        <v>5674</v>
+        <v>5526</v>
       </c>
       <c r="J65" s="25">
         <v>3000</v>
       </c>
       <c r="K65" s="25">
         <f t="shared" si="7"/>
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="L65" s="26">
         <f>I65/D65</f>
-        <v>1134.8</v>
+        <v>1842</v>
       </c>
       <c r="M65" s="25">
-        <v>35180</v>
+        <v>39074</v>
       </c>
       <c r="N65" s="25">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O65" s="25">
-        <v>502</v>
+        <v>456</v>
       </c>
       <c r="P65" s="25">
         <f>O65/I65</f>
-        <v>8.8473739866055695E-2</v>
+        <v>8.2519001085776325E-2</v>
       </c>
       <c r="Q65" s="26">
         <f>O65/D65</f>
-        <v>100.4</v>
+        <v>152</v>
       </c>
       <c r="R65" s="25">
-        <v>3110</v>
-      </c>
-    </row>
-    <row r="66" spans="2:18" s="25" customFormat="1">
+        <v>3226</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" s="25" customFormat="1">
+      <c r="A66" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="B66" s="25" t="s">
         <v>144</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D66" s="25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="F66" s="25" t="str">
         <f>LEFT(E66, 8)</f>
@@ -18005,279 +18013,1455 @@
         <v>0</v>
       </c>
       <c r="H66" s="25">
-        <v>24729</v>
+        <v>24643</v>
       </c>
       <c r="I66" s="25">
-        <v>6905</v>
+        <v>6154</v>
       </c>
       <c r="J66" s="25">
         <v>3000</v>
       </c>
       <c r="K66" s="25">
         <f t="shared" si="7"/>
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="L66" s="26">
         <f>I66/D66</f>
-        <v>1381</v>
+        <v>2051.3333333333335</v>
       </c>
       <c r="M66" s="25">
-        <v>36416</v>
+        <v>37504</v>
       </c>
       <c r="N66" s="25">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="O66" s="25">
-        <v>597</v>
+        <v>523</v>
       </c>
       <c r="P66" s="25">
         <f>O66/I66</f>
-        <v>8.6459087617668351E-2</v>
+        <v>8.4985375365615859E-2</v>
       </c>
       <c r="Q66" s="26">
         <f>O66/D66</f>
+        <v>174.33333333333334</v>
+      </c>
+      <c r="R66" s="25">
+        <v>3187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" s="5" customFormat="1">
+      <c r="L67" s="6"/>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:18">
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:18">
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="1:18">
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="1:18">
+      <c r="B72" t="s">
+        <v>251</v>
+      </c>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="1:18" s="38" customFormat="1">
+      <c r="B73" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D73" s="38">
+        <v>1</v>
+      </c>
+      <c r="E73" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="F73" s="38" t="str">
+        <f>LEFT(E73, 8)</f>
+        <v>20180813</v>
+      </c>
+      <c r="G73" s="38">
+        <v>0</v>
+      </c>
+      <c r="H73" s="38">
+        <v>3135</v>
+      </c>
+      <c r="I73" s="38">
+        <v>1742</v>
+      </c>
+      <c r="J73" s="38">
+        <v>400</v>
+      </c>
+      <c r="K73" s="38">
+        <f>J73/D73</f>
+        <v>400</v>
+      </c>
+      <c r="L73" s="39">
+        <f>I73/D73</f>
+        <v>1742</v>
+      </c>
+      <c r="M73" s="38">
+        <v>1605</v>
+      </c>
+      <c r="N73" s="38">
+        <v>109</v>
+      </c>
+      <c r="O73" s="38">
+        <v>293</v>
+      </c>
+      <c r="P73" s="38">
+        <f>O73/I73</f>
+        <v>0.16819747416762343</v>
+      </c>
+      <c r="Q73" s="39">
+        <f>O73/D73</f>
+        <v>293</v>
+      </c>
+      <c r="R73" s="38">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" s="38" customFormat="1">
+      <c r="B74" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D74" s="38">
+        <v>1</v>
+      </c>
+      <c r="E74" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="F74" s="38" t="str">
+        <f>LEFT(E74, 8)</f>
+        <v>20180813</v>
+      </c>
+      <c r="G74" s="38">
+        <v>0</v>
+      </c>
+      <c r="H74" s="38">
+        <v>2565</v>
+      </c>
+      <c r="I74" s="38">
+        <v>258</v>
+      </c>
+      <c r="J74" s="38">
+        <v>400</v>
+      </c>
+      <c r="K74" s="38">
+        <f t="shared" ref="K74:K96" si="8">J74/D74</f>
+        <v>400</v>
+      </c>
+      <c r="L74" s="39">
+        <f>I74/D74</f>
+        <v>258</v>
+      </c>
+      <c r="M74" s="38">
+        <v>972</v>
+      </c>
+      <c r="N74" s="38">
+        <v>27</v>
+      </c>
+      <c r="O74" s="38">
+        <v>44</v>
+      </c>
+      <c r="P74" s="38">
+        <f>O74/I74</f>
+        <v>0.17054263565891473</v>
+      </c>
+      <c r="Q74" s="39">
+        <f>O74/D74</f>
+        <v>44</v>
+      </c>
+      <c r="R74" s="38">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" s="38" customFormat="1">
+      <c r="B75" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D75" s="38">
+        <v>1</v>
+      </c>
+      <c r="E75" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="F75" s="38" t="str">
+        <f>LEFT(E75, 8)</f>
+        <v>20180813</v>
+      </c>
+      <c r="G75" s="38">
+        <v>0</v>
+      </c>
+      <c r="H75" s="38">
+        <v>2567</v>
+      </c>
+      <c r="I75" s="38">
+        <v>267</v>
+      </c>
+      <c r="J75" s="38">
+        <v>400</v>
+      </c>
+      <c r="K75" s="38">
+        <f t="shared" si="8"/>
+        <v>400</v>
+      </c>
+      <c r="L75" s="39">
+        <f>I75/D75</f>
+        <v>267</v>
+      </c>
+      <c r="M75" s="38">
+        <v>976</v>
+      </c>
+      <c r="N75" s="38">
+        <v>27</v>
+      </c>
+      <c r="O75" s="38">
+        <v>47</v>
+      </c>
+      <c r="P75" s="38">
+        <f>O75/I75</f>
+        <v>0.17602996254681649</v>
+      </c>
+      <c r="Q75" s="39">
+        <f>O75/D75</f>
+        <v>47</v>
+      </c>
+      <c r="R75" s="38">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" s="38" customFormat="1">
+      <c r="B76" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D76" s="38">
+        <v>1</v>
+      </c>
+      <c r="E76" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="F76" s="38" t="str">
+        <f>LEFT(E76, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G76" s="38">
+        <v>0</v>
+      </c>
+      <c r="H76" s="38">
+        <v>2551</v>
+      </c>
+      <c r="I76" s="38">
+        <v>255</v>
+      </c>
+      <c r="J76" s="38">
+        <v>400</v>
+      </c>
+      <c r="K76" s="38">
+        <f t="shared" si="8"/>
+        <v>400</v>
+      </c>
+      <c r="L76" s="39">
+        <f>I76/D76</f>
+        <v>255</v>
+      </c>
+      <c r="M76" s="38">
+        <v>954</v>
+      </c>
+      <c r="N76" s="38">
+        <v>27</v>
+      </c>
+      <c r="O76" s="38">
+        <v>43</v>
+      </c>
+      <c r="P76" s="38">
+        <f>O76/I76</f>
+        <v>0.16862745098039217</v>
+      </c>
+      <c r="Q76" s="39">
+        <f>O76/D76</f>
+        <v>43</v>
+      </c>
+      <c r="R76" s="38">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" s="38" customFormat="1">
+      <c r="B77" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D77" s="38">
+        <v>1</v>
+      </c>
+      <c r="E77" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="F77" s="38" t="str">
+        <f>LEFT(E77, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G77" s="38">
+        <v>0</v>
+      </c>
+      <c r="H77" s="38">
+        <v>2558</v>
+      </c>
+      <c r="I77" s="38">
+        <v>150</v>
+      </c>
+      <c r="J77" s="38">
+        <v>400</v>
+      </c>
+      <c r="K77" s="38">
+        <f t="shared" si="8"/>
+        <v>400</v>
+      </c>
+      <c r="L77" s="39">
+        <f>I77/D77</f>
+        <v>150</v>
+      </c>
+      <c r="M77" s="38">
+        <v>1018</v>
+      </c>
+      <c r="N77" s="38">
+        <v>15</v>
+      </c>
+      <c r="O77" s="38">
+        <v>26</v>
+      </c>
+      <c r="P77" s="38">
+        <f>O77/I77</f>
+        <v>0.17333333333333334</v>
+      </c>
+      <c r="Q77" s="39">
+        <f>O77/D77</f>
+        <v>26</v>
+      </c>
+      <c r="R77" s="38">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" s="38" customFormat="1">
+      <c r="B78" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C78" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D78" s="38">
+        <v>1</v>
+      </c>
+      <c r="E78" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="F78" s="38" t="str">
+        <f>LEFT(E78, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G78" s="38">
+        <v>0</v>
+      </c>
+      <c r="H78" s="38">
+        <v>2560</v>
+      </c>
+      <c r="I78" s="38">
+        <v>242</v>
+      </c>
+      <c r="J78" s="38">
+        <v>400</v>
+      </c>
+      <c r="K78" s="38">
+        <f t="shared" si="8"/>
+        <v>400</v>
+      </c>
+      <c r="L78" s="39">
+        <f>I78/D78</f>
+        <v>242</v>
+      </c>
+      <c r="M78" s="38">
+        <v>893</v>
+      </c>
+      <c r="N78" s="38">
+        <v>27</v>
+      </c>
+      <c r="O78" s="38">
+        <v>44</v>
+      </c>
+      <c r="P78" s="38">
+        <f>O78/I78</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="Q78" s="39">
+        <f>O78/D78</f>
+        <v>44</v>
+      </c>
+      <c r="R78" s="38">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" s="38" customFormat="1">
+      <c r="B79" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C79" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D79" s="38">
+        <v>1</v>
+      </c>
+      <c r="E79" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="F79" s="38" t="str">
+        <f>LEFT(E79, 8)</f>
+        <v>20180813</v>
+      </c>
+      <c r="G79" s="38">
+        <v>0</v>
+      </c>
+      <c r="H79" s="38">
+        <v>16498</v>
+      </c>
+      <c r="I79" s="38">
+        <v>3904</v>
+      </c>
+      <c r="J79" s="38">
+        <v>2000</v>
+      </c>
+      <c r="K79" s="38">
+        <f t="shared" si="8"/>
+        <v>2000</v>
+      </c>
+      <c r="L79" s="39">
+        <f>I79/D79</f>
+        <v>3904</v>
+      </c>
+      <c r="M79" s="38">
+        <v>23889</v>
+      </c>
+      <c r="N79" s="38">
+        <v>16</v>
+      </c>
+      <c r="O79" s="38">
+        <v>339</v>
+      </c>
+      <c r="P79" s="38">
+        <f>O79/I79</f>
+        <v>8.6834016393442626E-2</v>
+      </c>
+      <c r="Q79" s="39">
+        <f>O79/D79</f>
+        <v>339</v>
+      </c>
+      <c r="R79" s="38">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" s="38" customFormat="1">
+      <c r="B80" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D80" s="38">
+        <v>1</v>
+      </c>
+      <c r="E80" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="F80" s="38" t="str">
+        <f>LEFT(E80, 8)</f>
+        <v>20180813</v>
+      </c>
+      <c r="G80" s="38">
+        <v>0</v>
+      </c>
+      <c r="H80" s="38">
+        <v>16518</v>
+      </c>
+      <c r="I80" s="38">
+        <v>3496</v>
+      </c>
+      <c r="J80" s="38">
+        <v>2000</v>
+      </c>
+      <c r="K80" s="38">
+        <f t="shared" si="8"/>
+        <v>2000</v>
+      </c>
+      <c r="L80" s="39">
+        <f>I80/D80</f>
+        <v>3496</v>
+      </c>
+      <c r="M80" s="38">
+        <v>24308</v>
+      </c>
+      <c r="N80" s="38">
+        <v>14</v>
+      </c>
+      <c r="O80" s="38">
+        <v>303</v>
+      </c>
+      <c r="P80" s="38">
+        <f>O80/I80</f>
+        <v>8.6670480549199083E-2</v>
+      </c>
+      <c r="Q80" s="39">
+        <f>O80/D80</f>
+        <v>303</v>
+      </c>
+      <c r="R80" s="38">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="81" spans="2:18" s="38" customFormat="1">
+      <c r="B81" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C81" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D81" s="38">
+        <v>1</v>
+      </c>
+      <c r="E81" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="F81" s="38" t="str">
+        <f>LEFT(E81, 8)</f>
+        <v>20180813</v>
+      </c>
+      <c r="G81" s="38">
+        <v>0</v>
+      </c>
+      <c r="H81" s="38">
+        <v>17272</v>
+      </c>
+      <c r="I81" s="38">
+        <v>3445</v>
+      </c>
+      <c r="J81" s="38">
+        <v>2000</v>
+      </c>
+      <c r="K81" s="38">
+        <f t="shared" si="8"/>
+        <v>2000</v>
+      </c>
+      <c r="L81" s="39">
+        <f>I81/D81</f>
+        <v>3445</v>
+      </c>
+      <c r="M81" s="38">
+        <v>35363</v>
+      </c>
+      <c r="N81" s="38">
+        <v>10</v>
+      </c>
+      <c r="O81" s="38">
+        <v>250</v>
+      </c>
+      <c r="P81" s="38">
+        <f>O81/I81</f>
+        <v>7.2568940493468792E-2</v>
+      </c>
+      <c r="Q81" s="39">
+        <f>O81/D81</f>
+        <v>250</v>
+      </c>
+      <c r="R81" s="38">
+        <v>2572</v>
+      </c>
+    </row>
+    <row r="82" spans="2:18" s="38" customFormat="1">
+      <c r="B82" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C82" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="D82" s="38">
+        <v>1</v>
+      </c>
+      <c r="E82" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F82" s="38" t="str">
+        <f>LEFT(E82, 8)</f>
+        <v>20180813</v>
+      </c>
+      <c r="G82" s="38">
+        <v>0</v>
+      </c>
+      <c r="H82" s="38">
+        <v>36711</v>
+      </c>
+      <c r="I82" s="38">
+        <v>7585</v>
+      </c>
+      <c r="J82" s="38">
+        <v>4000</v>
+      </c>
+      <c r="K82" s="38">
+        <f t="shared" si="8"/>
+        <v>4000</v>
+      </c>
+      <c r="L82" s="39">
+        <f>I82/D82</f>
+        <v>7585</v>
+      </c>
+      <c r="M82" s="38">
+        <v>53502</v>
+      </c>
+      <c r="N82" s="38">
+        <v>14</v>
+      </c>
+      <c r="O82" s="38">
+        <v>661</v>
+      </c>
+      <c r="P82" s="38">
+        <f>O82/I82</f>
+        <v>8.7145682267633487E-2</v>
+      </c>
+      <c r="Q82" s="39">
+        <f>O82/D82</f>
+        <v>661</v>
+      </c>
+      <c r="R82" s="38">
+        <v>4666</v>
+      </c>
+    </row>
+    <row r="83" spans="2:18" s="38" customFormat="1">
+      <c r="B83" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C83" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="D83" s="38">
+        <v>1</v>
+      </c>
+      <c r="E83" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="F83" s="38" t="str">
+        <f>LEFT(E83, 8)</f>
+        <v>20180813</v>
+      </c>
+      <c r="G83" s="38">
+        <v>0</v>
+      </c>
+      <c r="H83" s="38">
+        <v>36717</v>
+      </c>
+      <c r="I83" s="38">
+        <v>7269</v>
+      </c>
+      <c r="J83" s="38">
+        <v>4000</v>
+      </c>
+      <c r="K83" s="38">
+        <f t="shared" si="8"/>
+        <v>4000</v>
+      </c>
+      <c r="L83" s="39">
+        <f>I83/D83</f>
+        <v>7269</v>
+      </c>
+      <c r="M83" s="38">
+        <v>52664</v>
+      </c>
+      <c r="N83" s="38">
+        <v>14</v>
+      </c>
+      <c r="O83" s="38">
+        <v>644</v>
+      </c>
+      <c r="P83" s="38">
+        <f>O83/I83</f>
+        <v>8.8595405145136877E-2</v>
+      </c>
+      <c r="Q83" s="39">
+        <f>O83/D83</f>
+        <v>644</v>
+      </c>
+      <c r="R83" s="38">
+        <v>4666</v>
+      </c>
+    </row>
+    <row r="84" spans="2:18" s="38" customFormat="1">
+      <c r="B84" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C84" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="D84" s="38">
+        <v>1</v>
+      </c>
+      <c r="E84" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="F84" s="38" t="str">
+        <f>LEFT(E84, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G84" s="38">
+        <v>0</v>
+      </c>
+      <c r="H84" s="38">
+        <v>36829</v>
+      </c>
+      <c r="I84" s="38">
+        <v>7396</v>
+      </c>
+      <c r="J84" s="38">
+        <v>4000</v>
+      </c>
+      <c r="K84" s="38">
+        <f t="shared" si="8"/>
+        <v>4000</v>
+      </c>
+      <c r="L84" s="39">
+        <f>I84/D84</f>
+        <v>7396</v>
+      </c>
+      <c r="M84" s="38">
+        <v>58227</v>
+      </c>
+      <c r="N84" s="38">
+        <v>13</v>
+      </c>
+      <c r="O84" s="38">
+        <v>621</v>
+      </c>
+      <c r="P84" s="38">
+        <f>O84/I84</f>
+        <v>8.3964305029745806E-2</v>
+      </c>
+      <c r="Q84" s="39">
+        <f>O84/D84</f>
+        <v>621</v>
+      </c>
+      <c r="R84" s="38">
+        <v>4896</v>
+      </c>
+    </row>
+    <row r="85" spans="2:18" s="38" customFormat="1">
+      <c r="B85" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C85" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D85" s="38">
+        <v>5</v>
+      </c>
+      <c r="E85" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="F85" s="38" t="str">
+        <f>LEFT(E85, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G85" s="38">
+        <v>0</v>
+      </c>
+      <c r="H85" s="38">
+        <v>23893</v>
+      </c>
+      <c r="I85" s="38">
+        <v>5864</v>
+      </c>
+      <c r="J85" s="38">
+        <v>3000</v>
+      </c>
+      <c r="K85" s="38">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="L85" s="39">
+        <f>I85/D85</f>
+        <v>1172.8</v>
+      </c>
+      <c r="M85" s="38">
+        <v>29547</v>
+      </c>
+      <c r="N85" s="38">
+        <v>20</v>
+      </c>
+      <c r="O85" s="38">
+        <v>555</v>
+      </c>
+      <c r="P85" s="38">
+        <f>O85/I85</f>
+        <v>9.464529331514325E-2</v>
+      </c>
+      <c r="Q85" s="39">
+        <f>O85/D85</f>
+        <v>111</v>
+      </c>
+      <c r="R85" s="38">
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="86" spans="2:18" s="38" customFormat="1">
+      <c r="B86" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C86" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D86" s="38">
+        <v>5</v>
+      </c>
+      <c r="E86" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="F86" s="38" t="str">
+        <f>LEFT(E86, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G86" s="38">
+        <v>0</v>
+      </c>
+      <c r="H86" s="38">
+        <v>24253</v>
+      </c>
+      <c r="I86" s="38">
+        <v>6137</v>
+      </c>
+      <c r="J86" s="38">
+        <v>3000</v>
+      </c>
+      <c r="K86" s="38">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="L86" s="39">
+        <f>I86/D86</f>
+        <v>1227.4000000000001</v>
+      </c>
+      <c r="M86" s="38">
+        <v>33525</v>
+      </c>
+      <c r="N86" s="38">
+        <v>18</v>
+      </c>
+      <c r="O86" s="38">
+        <v>562</v>
+      </c>
+      <c r="P86" s="38">
+        <f>O86/I86</f>
+        <v>9.1575688447124007E-2</v>
+      </c>
+      <c r="Q86" s="39">
+        <f>O86/D86</f>
+        <v>112.4</v>
+      </c>
+      <c r="R86" s="38">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="87" spans="2:18" s="38" customFormat="1">
+      <c r="B87" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C87" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D87" s="38">
+        <v>5</v>
+      </c>
+      <c r="E87" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="F87" s="38" t="str">
+        <f>LEFT(E87, 8)</f>
+        <v>20180815</v>
+      </c>
+      <c r="G87" s="38">
+        <v>0</v>
+      </c>
+      <c r="H87" s="38">
+        <v>24959</v>
+      </c>
+      <c r="I87" s="38">
+        <v>9892</v>
+      </c>
+      <c r="J87" s="38">
+        <v>3000</v>
+      </c>
+      <c r="K87" s="38">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="L87" s="39">
+        <f>I87/D87</f>
+        <v>1978.4</v>
+      </c>
+      <c r="M87" s="38">
+        <v>34604</v>
+      </c>
+      <c r="N87" s="38">
+        <v>29</v>
+      </c>
+      <c r="O87" s="38">
+        <v>879</v>
+      </c>
+      <c r="P87" s="38">
+        <f>O87/I87</f>
+        <v>8.8859684593611002E-2</v>
+      </c>
+      <c r="Q87" s="39">
+        <f>O87/D87</f>
+        <v>175.8</v>
+      </c>
+      <c r="R87" s="38">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="88" spans="2:18" s="38" customFormat="1">
+      <c r="B88" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C88" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D88" s="38">
+        <v>5</v>
+      </c>
+      <c r="E88" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="F88" s="38" t="str">
+        <f>LEFT(E88, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G88" s="38">
+        <v>0</v>
+      </c>
+      <c r="H88" s="38">
+        <v>24316</v>
+      </c>
+      <c r="I88" s="38">
+        <v>5809</v>
+      </c>
+      <c r="J88" s="38">
+        <v>3000</v>
+      </c>
+      <c r="K88" s="38">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="L88" s="39">
+        <f>I88/D88</f>
+        <v>1161.8</v>
+      </c>
+      <c r="M88" s="38">
+        <v>31070</v>
+      </c>
+      <c r="N88" s="38">
+        <v>19</v>
+      </c>
+      <c r="O88" s="38">
+        <v>552</v>
+      </c>
+      <c r="P88" s="38">
+        <f>O88/I88</f>
+        <v>9.5024961266999483E-2</v>
+      </c>
+      <c r="Q88" s="39">
+        <f>O88/D88</f>
+        <v>110.4</v>
+      </c>
+      <c r="R88" s="38">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="89" spans="2:18" s="38" customFormat="1">
+      <c r="B89" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C89" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D89" s="38">
+        <v>5</v>
+      </c>
+      <c r="E89" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="F89" s="38" t="str">
+        <f>LEFT(E89, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G89" s="38">
+        <v>0</v>
+      </c>
+      <c r="H89" s="38">
+        <v>24557</v>
+      </c>
+      <c r="I89" s="38">
+        <v>5725</v>
+      </c>
+      <c r="J89" s="38">
+        <v>3000</v>
+      </c>
+      <c r="K89" s="38">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="L89" s="39">
+        <f>I89/D89</f>
+        <v>1145</v>
+      </c>
+      <c r="M89" s="38">
+        <v>32726</v>
+      </c>
+      <c r="N89" s="38">
+        <v>17</v>
+      </c>
+      <c r="O89" s="38">
+        <v>524</v>
+      </c>
+      <c r="P89" s="38">
+        <f>O89/I89</f>
+        <v>9.1528384279475988E-2</v>
+      </c>
+      <c r="Q89" s="39">
+        <f>O89/D89</f>
+        <v>104.8</v>
+      </c>
+      <c r="R89" s="38">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="90" spans="2:18" s="38" customFormat="1">
+      <c r="B90" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C90" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D90" s="38">
+        <v>5</v>
+      </c>
+      <c r="E90" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="F90" s="38" t="str">
+        <f>LEFT(E90, 8)</f>
+        <v>20180815</v>
+      </c>
+      <c r="G90" s="38">
+        <v>0</v>
+      </c>
+      <c r="H90" s="38">
+        <v>24133</v>
+      </c>
+      <c r="I90" s="38">
+        <v>5796</v>
+      </c>
+      <c r="J90" s="38">
+        <v>3000</v>
+      </c>
+      <c r="K90" s="38">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="L90" s="39">
+        <f>I90/D90</f>
+        <v>1159.2</v>
+      </c>
+      <c r="M90" s="38">
+        <v>33081</v>
+      </c>
+      <c r="N90" s="38">
+        <v>18</v>
+      </c>
+      <c r="O90" s="38">
+        <v>532</v>
+      </c>
+      <c r="P90" s="38">
+        <f>O90/I90</f>
+        <v>9.1787439613526575E-2</v>
+      </c>
+      <c r="Q90" s="39">
+        <f>O90/D90</f>
+        <v>106.4</v>
+      </c>
+      <c r="R90" s="38">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="91" spans="2:18" s="38" customFormat="1">
+      <c r="B91" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C91" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="D91" s="38">
+        <v>5</v>
+      </c>
+      <c r="E91" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="F91" s="38" t="str">
+        <f>LEFT(E91, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G91" s="38">
+        <v>0</v>
+      </c>
+      <c r="H91" s="38">
+        <v>24475</v>
+      </c>
+      <c r="I91" s="38">
+        <v>5548</v>
+      </c>
+      <c r="J91" s="38">
+        <v>3000</v>
+      </c>
+      <c r="K91" s="38">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="L91" s="39">
+        <f>I91/D91</f>
+        <v>1109.5999999999999</v>
+      </c>
+      <c r="M91" s="38">
+        <v>36414</v>
+      </c>
+      <c r="N91" s="38">
+        <v>15</v>
+      </c>
+      <c r="O91" s="38">
+        <v>479</v>
+      </c>
+      <c r="P91" s="38">
+        <f>O91/I91</f>
+        <v>8.6337418889689974E-2</v>
+      </c>
+      <c r="Q91" s="39">
+        <f>O91/D91</f>
+        <v>95.8</v>
+      </c>
+      <c r="R91" s="38">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="92" spans="2:18" s="38" customFormat="1">
+      <c r="B92" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C92" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="D92" s="38">
+        <v>5</v>
+      </c>
+      <c r="E92" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="F92" s="38" t="str">
+        <f>LEFT(E92, 8)</f>
+        <v>20180814</v>
+      </c>
+      <c r="G92" s="38">
+        <v>0</v>
+      </c>
+      <c r="H92" s="38">
+        <v>24526</v>
+      </c>
+      <c r="I92" s="38">
+        <v>5674</v>
+      </c>
+      <c r="J92" s="38">
+        <v>3000</v>
+      </c>
+      <c r="K92" s="38">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="L92" s="39">
+        <f>I92/D92</f>
+        <v>1134.8</v>
+      </c>
+      <c r="M92" s="38">
+        <v>35180</v>
+      </c>
+      <c r="N92" s="38">
+        <v>16</v>
+      </c>
+      <c r="O92" s="38">
+        <v>502</v>
+      </c>
+      <c r="P92" s="38">
+        <f>O92/I92</f>
+        <v>8.8473739866055695E-2</v>
+      </c>
+      <c r="Q92" s="39">
+        <f>O92/D92</f>
+        <v>100.4</v>
+      </c>
+      <c r="R92" s="38">
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="93" spans="2:18" s="38" customFormat="1">
+      <c r="B93" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C93" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="D93" s="38">
+        <v>5</v>
+      </c>
+      <c r="E93" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="F93" s="38" t="str">
+        <f>LEFT(E93, 8)</f>
+        <v>20180815</v>
+      </c>
+      <c r="G93" s="38">
+        <v>0</v>
+      </c>
+      <c r="H93" s="38">
+        <v>24729</v>
+      </c>
+      <c r="I93" s="38">
+        <v>6905</v>
+      </c>
+      <c r="J93" s="38">
+        <v>3000</v>
+      </c>
+      <c r="K93" s="38">
+        <f t="shared" si="8"/>
+        <v>600</v>
+      </c>
+      <c r="L93" s="39">
+        <f>I93/D93</f>
+        <v>1381</v>
+      </c>
+      <c r="M93" s="38">
+        <v>36416</v>
+      </c>
+      <c r="N93" s="38">
+        <v>19</v>
+      </c>
+      <c r="O93" s="38">
+        <v>597</v>
+      </c>
+      <c r="P93" s="38">
+        <f>O93/I93</f>
+        <v>8.6459087617668351E-2</v>
+      </c>
+      <c r="Q93" s="39">
+        <f>O93/D93</f>
         <v>119.4</v>
       </c>
-      <c r="R66" s="25">
+      <c r="R93" s="38">
         <v>3149</v>
       </c>
     </row>
-    <row r="67" spans="2:18" s="25" customFormat="1">
-      <c r="B67" s="25" t="s">
+    <row r="94" spans="2:18" s="38" customFormat="1">
+      <c r="B94" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C94" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="D67" s="25">
+      <c r="D94" s="38">
         <v>3</v>
       </c>
-      <c r="E67" s="25" t="s">
+      <c r="E94" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="F67" s="25" t="str">
-        <f>LEFT(E67, 8)</f>
+      <c r="F94" s="38" t="str">
+        <f>LEFT(E94, 8)</f>
         <v>20180814</v>
       </c>
-      <c r="G67" s="25">
-        <v>0</v>
-      </c>
-      <c r="H67" s="25">
+      <c r="G94" s="38">
+        <v>0</v>
+      </c>
+      <c r="H94" s="38">
         <v>24831</v>
       </c>
-      <c r="I67" s="25">
+      <c r="I94" s="38">
         <v>5888</v>
       </c>
-      <c r="J67" s="25">
+      <c r="J94" s="38">
         <v>3000</v>
       </c>
-      <c r="K67" s="25">
-        <f t="shared" si="7"/>
+      <c r="K94" s="38">
+        <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="L67" s="26">
-        <f>I67/D67</f>
+      <c r="L94" s="39">
+        <f>I94/D94</f>
         <v>1962.6666666666667</v>
       </c>
-      <c r="M67" s="25">
+      <c r="M94" s="38">
         <v>37327</v>
       </c>
-      <c r="N67" s="25">
+      <c r="N94" s="38">
         <v>16</v>
       </c>
-      <c r="O67" s="25">
+      <c r="O94" s="38">
         <v>503</v>
       </c>
-      <c r="P67" s="25">
-        <f>O67/I67</f>
+      <c r="P94" s="38">
+        <f>O94/I94</f>
         <v>8.5427989130434784E-2</v>
       </c>
-      <c r="Q67" s="26">
-        <f>O67/D67</f>
+      <c r="Q94" s="39">
+        <f>O94/D94</f>
         <v>167.66666666666666</v>
       </c>
-      <c r="R67" s="25">
+      <c r="R94" s="38">
         <v>3187</v>
       </c>
     </row>
-    <row r="68" spans="2:18" s="25" customFormat="1">
-      <c r="B68" s="25" t="s">
+    <row r="95" spans="2:18" s="38" customFormat="1">
+      <c r="B95" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C95" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="25">
+      <c r="D95" s="38">
         <v>3</v>
       </c>
-      <c r="E68" s="25" t="s">
+      <c r="E95" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="F68" s="25" t="str">
-        <f>LEFT(E68, 8)</f>
+      <c r="F95" s="38" t="str">
+        <f>LEFT(E95, 8)</f>
         <v>20180814</v>
       </c>
-      <c r="G68" s="25">
-        <v>0</v>
-      </c>
-      <c r="H68" s="25">
+      <c r="G95" s="38">
+        <v>0</v>
+      </c>
+      <c r="H95" s="38">
         <v>24891</v>
       </c>
-      <c r="I68" s="25">
+      <c r="I95" s="38">
         <v>5526</v>
       </c>
-      <c r="J68" s="25">
+      <c r="J95" s="38">
         <v>3000</v>
       </c>
-      <c r="K68" s="25">
-        <f t="shared" si="7"/>
+      <c r="K95" s="38">
+        <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="L68" s="26">
-        <f>I68/D68</f>
+      <c r="L95" s="39">
+        <f>I95/D95</f>
         <v>1842</v>
       </c>
-      <c r="M68" s="25">
+      <c r="M95" s="38">
         <v>39074</v>
       </c>
-      <c r="N68" s="25">
+      <c r="N95" s="38">
         <v>14</v>
       </c>
-      <c r="O68" s="25">
+      <c r="O95" s="38">
         <v>456</v>
       </c>
-      <c r="P68" s="25">
-        <f>O68/I68</f>
+      <c r="P95" s="38">
+        <f>O95/I95</f>
         <v>8.2519001085776325E-2</v>
       </c>
-      <c r="Q68" s="26">
-        <f>O68/D68</f>
+      <c r="Q95" s="39">
+        <f>O95/D95</f>
         <v>152</v>
       </c>
-      <c r="R68" s="25">
+      <c r="R95" s="38">
         <v>3226</v>
       </c>
     </row>
-    <row r="69" spans="2:18" s="25" customFormat="1">
-      <c r="B69" s="25" t="s">
+    <row r="96" spans="2:18" s="38" customFormat="1">
+      <c r="B96" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="C69" s="25" t="s">
+      <c r="C96" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="D69" s="25">
+      <c r="D96" s="38">
         <v>3</v>
       </c>
-      <c r="E69" s="25" t="s">
+      <c r="E96" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="F69" s="25" t="str">
-        <f>LEFT(E69, 8)</f>
+      <c r="F96" s="38" t="str">
+        <f>LEFT(E96, 8)</f>
         <v>20180815</v>
       </c>
-      <c r="G69" s="25">
-        <v>0</v>
-      </c>
-      <c r="H69" s="25">
+      <c r="G96" s="38">
+        <v>0</v>
+      </c>
+      <c r="H96" s="38">
         <v>24643</v>
       </c>
-      <c r="I69" s="25">
+      <c r="I96" s="38">
         <v>6154</v>
       </c>
-      <c r="J69" s="25">
+      <c r="J96" s="38">
         <v>3000</v>
       </c>
-      <c r="K69" s="25">
-        <f t="shared" si="7"/>
+      <c r="K96" s="38">
+        <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="L69" s="26">
-        <f>I69/D69</f>
+      <c r="L96" s="39">
+        <f>I96/D96</f>
         <v>2051.3333333333335</v>
       </c>
-      <c r="M69" s="25">
+      <c r="M96" s="38">
         <v>37504</v>
       </c>
-      <c r="N69" s="25">
+      <c r="N96" s="38">
         <v>16</v>
       </c>
-      <c r="O69" s="25">
+      <c r="O96" s="38">
         <v>523</v>
       </c>
-      <c r="P69" s="25">
-        <f>O69/I69</f>
+      <c r="P96" s="38">
+        <f>O96/I96</f>
         <v>8.4985375365615859E-2</v>
       </c>
-      <c r="Q69" s="26">
-        <f>O69/D69</f>
+      <c r="Q96" s="39">
+        <f>O96/D96</f>
         <v>174.33333333333334</v>
       </c>
-      <c r="R69" s="25">
+      <c r="R96" s="38">
         <v>3187</v>
       </c>
-    </row>
-    <row r="70" spans="2:18" s="5" customFormat="1">
-      <c r="L70" s="6"/>
-    </row>
-    <row r="71" spans="2:18">
-      <c r="L71" s="2"/>
-    </row>
-    <row r="72" spans="2:18">
-      <c r="L72" s="2"/>
-    </row>
-    <row r="73" spans="2:18">
-      <c r="L73" s="2"/>
-    </row>
-    <row r="74" spans="2:18">
-      <c r="L74" s="2"/>
-    </row>
-    <row r="75" spans="2:18">
-      <c r="L75" s="2"/>
-    </row>
-    <row r="76" spans="2:18">
-      <c r="L76" s="2"/>
-    </row>
-    <row r="77" spans="2:18">
-      <c r="L77" s="2"/>
-    </row>
-    <row r="78" spans="2:18">
-      <c r="L78" s="2"/>
-    </row>
-    <row r="79" spans="2:18">
-      <c r="L79" s="2"/>
-    </row>
-    <row r="80" spans="2:18">
-      <c r="L80" s="2"/>
-    </row>
-    <row r="81" spans="12:12">
-      <c r="L81" s="2"/>
-    </row>
-    <row r="82" spans="12:12">
-      <c r="L82" s="2"/>
-    </row>
-    <row r="83" spans="12:12">
-      <c r="L83" s="2"/>
-    </row>
-    <row r="84" spans="12:12">
-      <c r="L84" s="2"/>
-    </row>
-    <row r="85" spans="12:12">
-      <c r="L85" s="2"/>
-    </row>
-    <row r="86" spans="12:12">
-      <c r="L86" s="2"/>
-    </row>
-    <row r="87" spans="12:12">
-      <c r="L87" s="2"/>
-    </row>
-    <row r="88" spans="12:12">
-      <c r="L88" s="2"/>
-    </row>
-    <row r="89" spans="12:12">
-      <c r="L89" s="2"/>
-    </row>
-    <row r="90" spans="12:12">
-      <c r="L90" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:S41" xr:uid="{201FADF2-299D-2E42-A643-0088FAFE31EF}">
@@ -18286,8 +19470,8 @@
       <sortCondition ref="C5:C41"/>
     </sortState>
   </autoFilter>
-  <sortState ref="B46:S57">
-    <sortCondition ref="E46:E57"/>
+  <sortState ref="B46:S54">
+    <sortCondition ref="E46:E54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18400,8 +19584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD3939F-B255-B24A-99D1-39EFD23212CB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18765,7 +19949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9321C540-539B-1E4C-910A-E4FA5307319D}">
   <dimension ref="B2:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -36934,7 +38118,7 @@
   <dimension ref="B3:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -37025,8 +38209,8 @@
         <v>141</v>
       </c>
       <c r="C9">
-        <f>CORREL(Results!I47:I57,Results!O47:O57)</f>
-        <v>0.99719040302191964</v>
+        <f>CORREL(Results!I46:I54,Results!O46:O54)</f>
+        <v>0.99951394853482556</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -37034,8 +38218,8 @@
         <v>163</v>
       </c>
       <c r="C10">
-        <f>CORREL(Results!K47:K57, Results!L47:L57)</f>
-        <v>0.99865410448320591</v>
+        <f>CORREL(Results!K47:K54, Results!L47:L54)</f>
+        <v>0.99649122497324194</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -37043,8 +38227,8 @@
         <v>162</v>
       </c>
       <c r="C11">
-        <f>CORREL(Results!K47:K57, Results!O47:O57)</f>
-        <v>0.99609087010734598</v>
+        <f>CORREL(Results!K47:K54, Results!O47:O54)</f>
+        <v>0.99670561243619415</v>
       </c>
     </row>
     <row r="12" spans="2:5">
@@ -37052,7 +38236,7 @@
         <v>164</v>
       </c>
       <c r="C12">
-        <f>CORREL(Results!K58:K69,Results!L58:L69)</f>
+        <f>CORREL(Results!K55:K66,Results!L55:L66)</f>
         <v>0.78791050738237067</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added rerun data test results
</commit_message>
<xml_diff>
--- a/Figures/TestResults.xlsx
+++ b/Figures/TestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eoin/Work/PhdThesis/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB8A81E-EA4E-C243-BC2B-3088CF960D72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8A9FB5-79C2-AD43-8019-929A5886B79C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="2880" windowWidth="27340" windowHeight="14440" xr2:uid="{BDA54389-B7CA-EC41-A61F-DEAE829EE646}"/>
+    <workbookView xWindow="640" yWindow="2820" windowWidth="27340" windowHeight="14440" firstSheet="1" activeTab="11" xr2:uid="{BDA54389-B7CA-EC41-A61F-DEAE829EE646}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{71F21A57-0D32-3642-ADCD-FAE884AA486B}" name="mpstat.allcpu" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/eoin/Work/EnergyApollo/data/single-cpu-x50-20180813-184337/mpstat.allcpu.txt" delimited="0">
+    <textPr sourceFile="/Users/eoin/Work/EnergyApollo/data/single-cpu-x50-20180813-184337/mpstat.allcpu.txt" delimited="0">
       <textFields count="12">
         <textField/>
         <textField position="11"/>
@@ -115,7 +115,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{D22E7628-3A3F-6D45-9B1C-34B2CC74B9A4}" name="pidstat.1stset" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/eoin/tmp/pidstat.1stset.txt" delimited="0">
+    <textPr sourceFile="/Users/eoin/tmp/pidstat.1stset.txt" delimited="0">
       <textFields count="13">
         <textField/>
         <textField position="13"/>
@@ -134,7 +134,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{AEA77F61-C93F-604C-A4D9-854E4A8A2C87}" name="pidstat.3278" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/eoin/Work/EnergyApollo/data/single-cpu-x50-20180813-184337/pidstat.3278.txt" delimited="0">
+    <textPr sourceFile="/Users/eoin/Work/EnergyApollo/data/single-cpu-x50-20180813-184337/pidstat.3278.txt" delimited="0">
       <textFields count="13">
         <textField/>
         <textField position="13"/>
@@ -153,7 +153,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{2C59186F-CBF5-504A-8AD8-21561081D470}" name="pidstat.3436" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/eoin/Work/EnergyApollo/data/single-cpu-x50-20180813-184337/pidstat.3436.txt" delimited="0">
+    <textPr sourceFile="/Users/eoin/Work/EnergyApollo/data/single-cpu-x50-20180813-184337/pidstat.3436.txt" delimited="0">
       <textFields count="14">
         <textField/>
         <textField position="12"/>
@@ -173,7 +173,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{C96270EA-BED8-1241-83F5-E29F52E710D0}" name="pidstat.3rdset" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/eoin/tmp/pidstat.3rdset.txt" delimited="0">
+    <textPr sourceFile="/Users/eoin/tmp/pidstat.3rdset.txt" delimited="0">
       <textFields count="13">
         <textField/>
         <textField position="13"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="275">
   <si>
     <t>Scenario</t>
   </si>
@@ -1001,7 +1001,43 @@
     <t>20180817-234858</t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>data-stdvolume-tests-20180817</t>
+  </si>
+  <si>
+    <t>20180818-001847</t>
+  </si>
+  <si>
+    <t>20180818-001952</t>
+  </si>
+  <si>
+    <t>20180818-002057</t>
+  </si>
+  <si>
+    <t>20180818-002203</t>
+  </si>
+  <si>
+    <t>20180818-002309</t>
+  </si>
+  <si>
+    <t>20180818-002415</t>
+  </si>
+  <si>
+    <t>20180818-002520</t>
+  </si>
+  <si>
+    <t>20180818-002626</t>
+  </si>
+  <si>
+    <t>20180818-002732</t>
+  </si>
+  <si>
+    <t>20180818-002838</t>
+  </si>
+  <si>
+    <t>20180818-002945</t>
+  </si>
+  <si>
+    <t>20180818-003051</t>
   </si>
 </sst>
 </file>
@@ -6373,6 +6409,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1031765663"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -7645,6 +7682,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1048781455"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -8348,6 +8386,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="974924143"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -8585,40 +8624,40 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1172.8</c:v>
+                  <c:v>1381.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1227.4000000000001</c:v>
+                  <c:v>1228.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1978.4</c:v>
+                  <c:v>1747</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1161.8</c:v>
+                  <c:v>1157.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1145</c:v>
+                  <c:v>1154.4000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1159.2</c:v>
+                  <c:v>1167.4000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1109.5999999999999</c:v>
+                  <c:v>1661.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1134.8</c:v>
+                  <c:v>1585</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1381</c:v>
+                  <c:v>1153.4000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1962.6666666666667</c:v>
+                  <c:v>1947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1842</c:v>
+                  <c:v>1910</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2051.3333333333335</c:v>
+                  <c:v>1993.3333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8715,40 +8754,40 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>111</c:v>
+                  <c:v>121.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>112.4</c:v>
+                  <c:v>114.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>175.8</c:v>
+                  <c:v>151.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.4</c:v>
+                  <c:v>109.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>104.8</c:v>
+                  <c:v>107.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>106.4</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>95.8</c:v>
+                  <c:v>142.80000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100.4</c:v>
+                  <c:v>136.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>119.4</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>167.66666666666666</c:v>
+                  <c:v>163.33333333333334</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>152</c:v>
+                  <c:v>157.33333333333334</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>174.33333333333334</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8960,6 +8999,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1103591567"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -14618,11 +14658,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A7A84C-38BB-9C46-BB61-734C431F3DDA}">
-  <dimension ref="A2:S96"/>
+  <dimension ref="B2:S96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55:A66"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16249,7 +16289,7 @@
         <v>70</v>
       </c>
       <c r="F35" s="9" t="str">
-        <f t="shared" ref="F35:F54" si="6">LEFT(E35, 8)</f>
+        <f t="shared" ref="F35:F45" si="6">LEFT(E35, 8)</f>
         <v>20180808</v>
       </c>
       <c r="G35" s="7">
@@ -16810,7 +16850,7 @@
         <v>254</v>
       </c>
       <c r="F46" s="23" t="str">
-        <f>LEFT(E46, 8)</f>
+        <f t="shared" ref="F46:F66" si="7">LEFT(E46, 8)</f>
         <v>20180817</v>
       </c>
       <c r="G46" s="23">
@@ -16826,11 +16866,11 @@
         <v>400</v>
       </c>
       <c r="K46" s="23">
-        <f>J46/D46</f>
+        <f t="shared" ref="K46:K54" si="8">J46/D46</f>
         <v>400</v>
       </c>
       <c r="L46" s="24">
-        <f>I46/D46</f>
+        <f t="shared" ref="L46:L66" si="9">I46/D46</f>
         <v>188</v>
       </c>
       <c r="M46" s="23">
@@ -16843,11 +16883,11 @@
         <v>44</v>
       </c>
       <c r="P46" s="23">
-        <f>O46/I46</f>
+        <f t="shared" ref="P46:P66" si="10">O46/I46</f>
         <v>0.23404255319148937</v>
       </c>
       <c r="Q46" s="24">
-        <f>O46/D46</f>
+        <f t="shared" ref="Q46:Q66" si="11">O46/D46</f>
         <v>44</v>
       </c>
       <c r="R46" s="23">
@@ -16868,7 +16908,7 @@
         <v>255</v>
       </c>
       <c r="F47" s="23" t="str">
-        <f>LEFT(E47, 8)</f>
+        <f t="shared" si="7"/>
         <v>20180817</v>
       </c>
       <c r="G47" s="23">
@@ -16884,11 +16924,11 @@
         <v>400</v>
       </c>
       <c r="K47" s="23">
-        <f>J47/D47</f>
+        <f t="shared" si="8"/>
         <v>400</v>
       </c>
       <c r="L47" s="24">
-        <f>I47/D47</f>
+        <f t="shared" si="9"/>
         <v>276</v>
       </c>
       <c r="M47" s="23">
@@ -16901,11 +16941,11 @@
         <v>45</v>
       </c>
       <c r="P47" s="23">
-        <f>O47/I47</f>
+        <f t="shared" si="10"/>
         <v>0.16304347826086957</v>
       </c>
       <c r="Q47" s="24">
-        <f>O47/D47</f>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="R47" s="23">
@@ -16926,7 +16966,7 @@
         <v>256</v>
       </c>
       <c r="F48" s="23" t="str">
-        <f>LEFT(E48, 8)</f>
+        <f t="shared" si="7"/>
         <v>20180817</v>
       </c>
       <c r="G48" s="23">
@@ -16942,11 +16982,11 @@
         <v>400</v>
       </c>
       <c r="K48" s="23">
-        <f>J48/D48</f>
+        <f t="shared" si="8"/>
         <v>400</v>
       </c>
       <c r="L48" s="24">
-        <f>I48/D48</f>
+        <f t="shared" si="9"/>
         <v>279</v>
       </c>
       <c r="M48" s="23">
@@ -16959,18 +16999,18 @@
         <v>48</v>
       </c>
       <c r="P48" s="23">
-        <f>O48/I48</f>
+        <f t="shared" si="10"/>
         <v>0.17204301075268819</v>
       </c>
       <c r="Q48" s="24">
-        <f>O48/D48</f>
+        <f t="shared" si="11"/>
         <v>48</v>
       </c>
       <c r="R48" s="23">
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:18" s="23" customFormat="1">
+    <row r="49" spans="2:18" s="23" customFormat="1">
       <c r="B49" s="23" t="s">
         <v>252</v>
       </c>
@@ -16984,7 +17024,7 @@
         <v>260</v>
       </c>
       <c r="F49" s="23" t="str">
-        <f>LEFT(E49, 8)</f>
+        <f t="shared" si="7"/>
         <v>20180817</v>
       </c>
       <c r="G49" s="23">
@@ -17000,11 +17040,11 @@
         <v>2000</v>
       </c>
       <c r="K49" s="23">
-        <f>J49/D49</f>
+        <f t="shared" si="8"/>
         <v>2000</v>
       </c>
       <c r="L49" s="24">
-        <f>I49/D49</f>
+        <f t="shared" si="9"/>
         <v>3282</v>
       </c>
       <c r="M49" s="23">
@@ -17017,18 +17057,18 @@
         <v>285</v>
       </c>
       <c r="P49" s="23">
-        <f>O49/I49</f>
+        <f t="shared" si="10"/>
         <v>8.6837294332723955E-2</v>
       </c>
       <c r="Q49" s="24">
-        <f>O49/D49</f>
+        <f t="shared" si="11"/>
         <v>285</v>
       </c>
       <c r="R49" s="23">
         <v>2099</v>
       </c>
     </row>
-    <row r="50" spans="1:18" s="23" customFormat="1">
+    <row r="50" spans="2:18" s="23" customFormat="1">
       <c r="B50" s="23" t="s">
         <v>252</v>
       </c>
@@ -17042,7 +17082,7 @@
         <v>261</v>
       </c>
       <c r="F50" s="23" t="str">
-        <f>LEFT(E50, 8)</f>
+        <f t="shared" si="7"/>
         <v>20180817</v>
       </c>
       <c r="G50" s="23">
@@ -17058,11 +17098,11 @@
         <v>2000</v>
       </c>
       <c r="K50" s="23">
-        <f>J50/D50</f>
+        <f t="shared" si="8"/>
         <v>2000</v>
       </c>
       <c r="L50" s="24">
-        <f>I50/D50</f>
+        <f t="shared" si="9"/>
         <v>3648</v>
       </c>
       <c r="M50" s="23">
@@ -17075,18 +17115,18 @@
         <v>320</v>
       </c>
       <c r="P50" s="23">
-        <f>O50/I50</f>
+        <f t="shared" si="10"/>
         <v>8.771929824561403E-2</v>
       </c>
       <c r="Q50" s="24">
-        <f>O50/D50</f>
+        <f t="shared" si="11"/>
         <v>320</v>
       </c>
       <c r="R50" s="23">
         <v>2048</v>
       </c>
     </row>
-    <row r="51" spans="1:18" s="23" customFormat="1">
+    <row r="51" spans="2:18" s="23" customFormat="1">
       <c r="B51" s="23" t="s">
         <v>252</v>
       </c>
@@ -17100,7 +17140,7 @@
         <v>253</v>
       </c>
       <c r="F51" s="23" t="str">
-        <f>LEFT(E51, 8)</f>
+        <f t="shared" si="7"/>
         <v>20180817</v>
       </c>
       <c r="G51" s="23">
@@ -17116,11 +17156,11 @@
         <v>2000</v>
       </c>
       <c r="K51" s="23">
-        <f>J51/D51</f>
+        <f t="shared" si="8"/>
         <v>2000</v>
       </c>
       <c r="L51" s="24">
-        <f>I51/D51</f>
+        <f t="shared" si="9"/>
         <v>3523</v>
       </c>
       <c r="M51" s="23">
@@ -17133,18 +17173,18 @@
         <v>328</v>
       </c>
       <c r="P51" s="23">
-        <f>O51/I51</f>
+        <f t="shared" si="10"/>
         <v>9.3102469486233325E-2</v>
       </c>
       <c r="Q51" s="24">
-        <f>O51/D51</f>
+        <f t="shared" si="11"/>
         <v>328</v>
       </c>
       <c r="R51" s="23">
         <v>1971</v>
       </c>
     </row>
-    <row r="52" spans="1:18" s="23" customFormat="1">
+    <row r="52" spans="2:18" s="23" customFormat="1">
       <c r="B52" s="23" t="s">
         <v>252</v>
       </c>
@@ -17158,7 +17198,7 @@
         <v>257</v>
       </c>
       <c r="F52" s="23" t="str">
-        <f>LEFT(E52, 8)</f>
+        <f t="shared" si="7"/>
         <v>20180817</v>
       </c>
       <c r="G52" s="23">
@@ -17174,11 +17214,11 @@
         <v>4000</v>
       </c>
       <c r="K52" s="23">
-        <f>J52/D52</f>
+        <f t="shared" si="8"/>
         <v>4000</v>
       </c>
       <c r="L52" s="24">
-        <f>I52/D52</f>
+        <f t="shared" si="9"/>
         <v>8541</v>
       </c>
       <c r="M52" s="23">
@@ -17191,18 +17231,18 @@
         <v>707</v>
       </c>
       <c r="P52" s="23">
-        <f>O52/I52</f>
+        <f t="shared" si="10"/>
         <v>8.277719236623346E-2</v>
       </c>
       <c r="Q52" s="24">
-        <f>O52/D52</f>
+        <f t="shared" si="11"/>
         <v>707</v>
       </c>
       <c r="R52" s="23">
         <v>4946</v>
       </c>
     </row>
-    <row r="53" spans="1:18" s="23" customFormat="1">
+    <row r="53" spans="2:18" s="23" customFormat="1">
       <c r="B53" s="23" t="s">
         <v>252</v>
       </c>
@@ -17216,7 +17256,7 @@
         <v>258</v>
       </c>
       <c r="F53" s="23" t="str">
-        <f>LEFT(E53, 8)</f>
+        <f t="shared" si="7"/>
         <v>20180817</v>
       </c>
       <c r="G53" s="23">
@@ -17232,11 +17272,11 @@
         <v>4000</v>
       </c>
       <c r="K53" s="23">
-        <f>J53/D53</f>
+        <f t="shared" si="8"/>
         <v>4000</v>
       </c>
       <c r="L53" s="24">
-        <f>I53/D53</f>
+        <f t="shared" si="9"/>
         <v>8265</v>
       </c>
       <c r="M53" s="23">
@@ -17249,18 +17289,18 @@
         <v>671</v>
       </c>
       <c r="P53" s="23">
-        <f>O53/I53</f>
+        <f t="shared" si="10"/>
         <v>8.1185722928009685E-2</v>
       </c>
       <c r="Q53" s="24">
-        <f>O53/D53</f>
+        <f t="shared" si="11"/>
         <v>671</v>
       </c>
       <c r="R53" s="23">
         <v>4946</v>
       </c>
     </row>
-    <row r="54" spans="1:18" s="23" customFormat="1">
+    <row r="54" spans="2:18" s="23" customFormat="1">
       <c r="B54" s="23" t="s">
         <v>252</v>
       </c>
@@ -17274,7 +17314,7 @@
         <v>259</v>
       </c>
       <c r="F54" s="23" t="str">
-        <f>LEFT(E54, 8)</f>
+        <f t="shared" si="7"/>
         <v>20180817</v>
       </c>
       <c r="G54" s="23">
@@ -17290,11 +17330,11 @@
         <v>4000</v>
       </c>
       <c r="K54" s="23">
-        <f>J54/D54</f>
+        <f t="shared" si="8"/>
         <v>4000</v>
       </c>
       <c r="L54" s="24">
-        <f>I54/D54</f>
+        <f t="shared" si="9"/>
         <v>8820</v>
       </c>
       <c r="M54" s="23">
@@ -17307,23 +17347,20 @@
         <v>721</v>
       </c>
       <c r="P54" s="23">
-        <f>O54/I54</f>
+        <f t="shared" si="10"/>
         <v>8.1746031746031747E-2</v>
       </c>
       <c r="Q54" s="24">
-        <f>O54/D54</f>
+        <f t="shared" si="11"/>
         <v>721</v>
       </c>
       <c r="R54" s="23">
         <v>4946</v>
       </c>
     </row>
-    <row r="55" spans="1:18" s="25" customFormat="1">
-      <c r="A55" s="25" t="s">
+    <row r="55" spans="2:18" s="25" customFormat="1">
+      <c r="B55" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C55" s="25" t="s">
         <v>147</v>
@@ -17332,59 +17369,56 @@
         <v>5</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>148</v>
+        <v>263</v>
       </c>
       <c r="F55" s="25" t="str">
-        <f>LEFT(E55, 8)</f>
-        <v>20180814</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G55" s="25">
         <v>0</v>
       </c>
       <c r="H55" s="25">
-        <v>23893</v>
+        <v>23895</v>
       </c>
       <c r="I55" s="25">
-        <v>5864</v>
+        <v>6908</v>
       </c>
       <c r="J55" s="25">
         <v>3000</v>
       </c>
       <c r="K55" s="25">
-        <f t="shared" ref="K47:K66" si="7">J55/D55</f>
+        <f t="shared" ref="K55:K66" si="12">J55/D55</f>
         <v>600</v>
       </c>
       <c r="L55" s="26">
-        <f>I55/D55</f>
-        <v>1172.8</v>
+        <f t="shared" si="9"/>
+        <v>1381.6</v>
       </c>
       <c r="M55" s="25">
-        <v>29547</v>
+        <v>33498</v>
       </c>
       <c r="N55" s="25">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O55" s="25">
-        <v>555</v>
+        <v>607</v>
       </c>
       <c r="P55" s="25">
-        <f>O55/I55</f>
-        <v>9.464529331514325E-2</v>
+        <f t="shared" si="10"/>
+        <v>8.7869137232194555E-2</v>
       </c>
       <c r="Q55" s="26">
-        <f>O55/D55</f>
-        <v>111</v>
+        <f t="shared" si="11"/>
+        <v>121.4</v>
       </c>
       <c r="R55" s="25">
-        <v>2797</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" s="25" customFormat="1">
-      <c r="A56" s="25" t="s">
+        <v>2944</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18" s="25" customFormat="1">
+      <c r="B56" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>147</v>
@@ -17393,59 +17427,56 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>149</v>
+        <v>264</v>
       </c>
       <c r="F56" s="25" t="str">
-        <f>LEFT(E56, 8)</f>
-        <v>20180814</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G56" s="25">
         <v>0</v>
       </c>
       <c r="H56" s="25">
-        <v>24253</v>
+        <v>24030</v>
       </c>
       <c r="I56" s="25">
-        <v>6137</v>
+        <v>6141</v>
       </c>
       <c r="J56" s="25">
         <v>3000</v>
       </c>
       <c r="K56" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="L56" s="26">
-        <f>I56/D56</f>
-        <v>1227.4000000000001</v>
+        <f t="shared" si="9"/>
+        <v>1228.2</v>
       </c>
       <c r="M56" s="25">
-        <v>33525</v>
+        <v>32127</v>
       </c>
       <c r="N56" s="25">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O56" s="25">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="P56" s="25">
-        <f>O56/I56</f>
-        <v>9.1575688447124007E-2</v>
+        <f t="shared" si="10"/>
+        <v>9.3144439016446839E-2</v>
       </c>
       <c r="Q56" s="26">
-        <f>O56/D56</f>
-        <v>112.4</v>
+        <f t="shared" si="11"/>
+        <v>114.4</v>
       </c>
       <c r="R56" s="25">
-        <v>3072</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" s="25" customFormat="1">
-      <c r="A57" s="25" t="s">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" s="25" customFormat="1">
+      <c r="B57" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C57" s="25" t="s">
         <v>147</v>
@@ -17454,59 +17485,56 @@
         <v>5</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>150</v>
+        <v>265</v>
       </c>
       <c r="F57" s="25" t="str">
-        <f>LEFT(E57, 8)</f>
-        <v>20180815</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G57" s="25">
         <v>0</v>
       </c>
       <c r="H57" s="25">
-        <v>24959</v>
+        <v>23966</v>
       </c>
       <c r="I57" s="25">
-        <v>9892</v>
+        <v>8735</v>
       </c>
       <c r="J57" s="25">
         <v>3000</v>
       </c>
       <c r="K57" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="L57" s="26">
-        <f>I57/D57</f>
-        <v>1978.4</v>
+        <f t="shared" si="9"/>
+        <v>1747</v>
       </c>
       <c r="M57" s="25">
-        <v>34604</v>
+        <v>34376</v>
       </c>
       <c r="N57" s="25">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="O57" s="25">
-        <v>879</v>
+        <v>757</v>
       </c>
       <c r="P57" s="25">
-        <f>O57/I57</f>
-        <v>8.8859684593611002E-2</v>
+        <f t="shared" si="10"/>
+        <v>8.6662850601030336E-2</v>
       </c>
       <c r="Q57" s="26">
-        <f>O57/D57</f>
-        <v>175.8</v>
+        <f t="shared" si="11"/>
+        <v>151.4</v>
       </c>
       <c r="R57" s="25">
-        <v>3072</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" s="25" customFormat="1">
-      <c r="A58" s="25" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" s="25" customFormat="1">
+      <c r="B58" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C58" s="25" t="s">
         <v>151</v>
@@ -17515,59 +17543,56 @@
         <v>5</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>152</v>
+        <v>266</v>
       </c>
       <c r="F58" s="25" t="str">
-        <f>LEFT(E58, 8)</f>
-        <v>20180814</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G58" s="25">
         <v>0</v>
       </c>
       <c r="H58" s="25">
-        <v>24316</v>
+        <v>24235</v>
       </c>
       <c r="I58" s="25">
-        <v>5809</v>
+        <v>5786</v>
       </c>
       <c r="J58" s="25">
         <v>3000</v>
       </c>
       <c r="K58" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="L58" s="26">
-        <f>I58/D58</f>
-        <v>1161.8</v>
+        <f t="shared" si="9"/>
+        <v>1157.2</v>
       </c>
       <c r="M58" s="25">
-        <v>31070</v>
+        <v>31625</v>
       </c>
       <c r="N58" s="25">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O58" s="25">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="P58" s="25">
-        <f>O58/I58</f>
-        <v>9.5024961266999483E-2</v>
+        <f t="shared" si="10"/>
+        <v>9.4711372277912195E-2</v>
       </c>
       <c r="Q58" s="26">
-        <f>O58/D58</f>
-        <v>110.4</v>
+        <f t="shared" si="11"/>
+        <v>109.6</v>
       </c>
       <c r="R58" s="25">
-        <v>2957</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" s="25" customFormat="1">
-      <c r="A59" s="25" t="s">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" s="25" customFormat="1">
+      <c r="B59" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>151</v>
@@ -17576,59 +17601,56 @@
         <v>5</v>
       </c>
       <c r="E59" s="25" t="s">
-        <v>153</v>
+        <v>267</v>
       </c>
       <c r="F59" s="25" t="str">
-        <f>LEFT(E59, 8)</f>
-        <v>20180814</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G59" s="25">
         <v>0</v>
       </c>
       <c r="H59" s="25">
-        <v>24557</v>
+        <v>24311</v>
       </c>
       <c r="I59" s="25">
-        <v>5725</v>
+        <v>5772</v>
       </c>
       <c r="J59" s="25">
         <v>3000</v>
       </c>
       <c r="K59" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="L59" s="26">
-        <f>I59/D59</f>
-        <v>1145</v>
+        <f t="shared" si="9"/>
+        <v>1154.4000000000001</v>
       </c>
       <c r="M59" s="25">
-        <v>32726</v>
+        <v>32169</v>
       </c>
       <c r="N59" s="25">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O59" s="25">
-        <v>524</v>
+        <v>537</v>
       </c>
       <c r="P59" s="25">
-        <f>O59/I59</f>
-        <v>9.1528384279475988E-2</v>
+        <f t="shared" si="10"/>
+        <v>9.3035343035343041E-2</v>
       </c>
       <c r="Q59" s="26">
-        <f>O59/D59</f>
-        <v>104.8</v>
+        <f t="shared" si="11"/>
+        <v>107.4</v>
       </c>
       <c r="R59" s="25">
         <v>2995</v>
       </c>
     </row>
-    <row r="60" spans="1:18" s="25" customFormat="1">
-      <c r="A60" s="25" t="s">
+    <row r="60" spans="2:18" s="25" customFormat="1">
+      <c r="B60" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>151</v>
@@ -17637,59 +17659,56 @@
         <v>5</v>
       </c>
       <c r="E60" s="25" t="s">
-        <v>154</v>
+        <v>268</v>
       </c>
       <c r="F60" s="25" t="str">
-        <f>LEFT(E60, 8)</f>
-        <v>20180815</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G60" s="25">
         <v>0</v>
       </c>
       <c r="H60" s="25">
-        <v>24133</v>
+        <v>24291</v>
       </c>
       <c r="I60" s="25">
-        <v>5796</v>
+        <v>5837</v>
       </c>
       <c r="J60" s="25">
         <v>3000</v>
       </c>
       <c r="K60" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="L60" s="26">
-        <f>I60/D60</f>
-        <v>1159.2</v>
+        <f t="shared" si="9"/>
+        <v>1167.4000000000001</v>
       </c>
       <c r="M60" s="25">
-        <v>33081</v>
+        <v>33387</v>
       </c>
       <c r="N60" s="25">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O60" s="25">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="P60" s="25">
-        <f>O60/I60</f>
-        <v>9.1787439613526575E-2</v>
+        <f t="shared" si="10"/>
+        <v>9.0800068528353609E-2</v>
       </c>
       <c r="Q60" s="26">
-        <f>O60/D60</f>
-        <v>106.4</v>
+        <f t="shared" si="11"/>
+        <v>106</v>
       </c>
       <c r="R60" s="25">
         <v>3034</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="25" customFormat="1">
-      <c r="A61" s="25" t="s">
+    <row r="61" spans="2:18" s="25" customFormat="1">
+      <c r="B61" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B61" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>155</v>
@@ -17698,59 +17717,56 @@
         <v>5</v>
       </c>
       <c r="E61" s="25" t="s">
-        <v>156</v>
+        <v>269</v>
       </c>
       <c r="F61" s="25" t="str">
-        <f>LEFT(E61, 8)</f>
-        <v>20180814</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G61" s="25">
         <v>0</v>
       </c>
       <c r="H61" s="25">
-        <v>24475</v>
+        <v>24401</v>
       </c>
       <c r="I61" s="25">
-        <v>5548</v>
+        <v>8309</v>
       </c>
       <c r="J61" s="25">
         <v>3000</v>
       </c>
       <c r="K61" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="L61" s="26">
-        <f>I61/D61</f>
-        <v>1109.5999999999999</v>
+        <f t="shared" si="9"/>
+        <v>1661.8</v>
       </c>
       <c r="M61" s="25">
-        <v>36414</v>
+        <v>37088</v>
       </c>
       <c r="N61" s="25">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="O61" s="25">
-        <v>479</v>
+        <v>714</v>
       </c>
       <c r="P61" s="25">
-        <f>O61/I61</f>
-        <v>8.6337418889689974E-2</v>
+        <f t="shared" si="10"/>
+        <v>8.5930918281381635E-2</v>
       </c>
       <c r="Q61" s="26">
-        <f>O61/D61</f>
-        <v>95.8</v>
+        <f t="shared" si="11"/>
+        <v>142.80000000000001</v>
       </c>
       <c r="R61" s="25">
-        <v>3149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" s="25" customFormat="1">
-      <c r="A62" s="25" t="s">
+        <v>3187</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" s="25" customFormat="1">
+      <c r="B62" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>155</v>
@@ -17759,59 +17775,56 @@
         <v>5</v>
       </c>
       <c r="E62" s="25" t="s">
-        <v>157</v>
+        <v>270</v>
       </c>
       <c r="F62" s="25" t="str">
-        <f>LEFT(E62, 8)</f>
-        <v>20180814</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G62" s="25">
         <v>0</v>
       </c>
       <c r="H62" s="25">
-        <v>24526</v>
+        <v>24524</v>
       </c>
       <c r="I62" s="25">
-        <v>5674</v>
+        <v>7925</v>
       </c>
       <c r="J62" s="25">
         <v>3000</v>
       </c>
       <c r="K62" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="L62" s="26">
-        <f>I62/D62</f>
-        <v>1134.8</v>
+        <f t="shared" si="9"/>
+        <v>1585</v>
       </c>
       <c r="M62" s="25">
-        <v>35180</v>
+        <v>37071</v>
       </c>
       <c r="N62" s="25">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="O62" s="25">
-        <v>502</v>
+        <v>681</v>
       </c>
       <c r="P62" s="25">
-        <f>O62/I62</f>
-        <v>8.8473739866055695E-2</v>
+        <f t="shared" si="10"/>
+        <v>8.5930599369085175E-2</v>
       </c>
       <c r="Q62" s="26">
-        <f>O62/D62</f>
-        <v>100.4</v>
+        <f t="shared" si="11"/>
+        <v>136.19999999999999</v>
       </c>
       <c r="R62" s="25">
-        <v>3110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" s="25" customFormat="1">
-      <c r="A63" s="25" t="s">
+        <v>3187</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" s="25" customFormat="1">
+      <c r="B63" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B63" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>155</v>
@@ -17820,59 +17833,56 @@
         <v>5</v>
       </c>
       <c r="E63" s="25" t="s">
-        <v>158</v>
+        <v>271</v>
       </c>
       <c r="F63" s="25" t="str">
-        <f>LEFT(E63, 8)</f>
-        <v>20180815</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G63" s="25">
         <v>0</v>
       </c>
       <c r="H63" s="25">
-        <v>24729</v>
+        <v>24408</v>
       </c>
       <c r="I63" s="25">
-        <v>6905</v>
+        <v>5767</v>
       </c>
       <c r="J63" s="25">
         <v>3000</v>
       </c>
       <c r="K63" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="L63" s="26">
-        <f>I63/D63</f>
-        <v>1381</v>
+        <f t="shared" si="9"/>
+        <v>1153.4000000000001</v>
       </c>
       <c r="M63" s="25">
-        <v>36416</v>
+        <v>33316</v>
       </c>
       <c r="N63" s="25">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O63" s="25">
-        <v>597</v>
+        <v>525</v>
       </c>
       <c r="P63" s="25">
-        <f>O63/I63</f>
-        <v>8.6459087617668351E-2</v>
+        <f t="shared" si="10"/>
+        <v>9.1035200277440609E-2</v>
       </c>
       <c r="Q63" s="26">
-        <f>O63/D63</f>
-        <v>119.4</v>
+        <f t="shared" si="11"/>
+        <v>105</v>
       </c>
       <c r="R63" s="25">
-        <v>3149</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" s="25" customFormat="1">
-      <c r="A64" s="25" t="s">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="64" spans="2:18" s="25" customFormat="1">
+      <c r="B64" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B64" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>145</v>
@@ -17881,59 +17891,56 @@
         <v>3</v>
       </c>
       <c r="E64" s="25" t="s">
-        <v>159</v>
+        <v>272</v>
       </c>
       <c r="F64" s="25" t="str">
-        <f>LEFT(E64, 8)</f>
-        <v>20180814</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G64" s="25">
         <v>0</v>
       </c>
       <c r="H64" s="25">
-        <v>24831</v>
+        <v>24793</v>
       </c>
       <c r="I64" s="25">
-        <v>5888</v>
+        <v>5841</v>
       </c>
       <c r="J64" s="25">
         <v>3000</v>
       </c>
       <c r="K64" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1000</v>
       </c>
       <c r="L64" s="26">
-        <f>I64/D64</f>
-        <v>1962.6666666666667</v>
+        <f t="shared" si="9"/>
+        <v>1947</v>
       </c>
       <c r="M64" s="25">
-        <v>37327</v>
+        <v>38487</v>
       </c>
       <c r="N64" s="25">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O64" s="25">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="P64" s="25">
-        <f>O64/I64</f>
-        <v>8.5427989130434784E-2</v>
+        <f t="shared" si="10"/>
+        <v>8.3889744906694055E-2</v>
       </c>
       <c r="Q64" s="26">
-        <f>O64/D64</f>
-        <v>167.66666666666666</v>
+        <f t="shared" si="11"/>
+        <v>163.33333333333334</v>
       </c>
       <c r="R64" s="25">
-        <v>3187</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" s="25" customFormat="1">
-      <c r="A65" s="25" t="s">
+        <v>3226</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" s="25" customFormat="1">
+      <c r="B65" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B65" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C65" s="25" t="s">
         <v>145</v>
@@ -17942,59 +17949,56 @@
         <v>3</v>
       </c>
       <c r="E65" s="25" t="s">
-        <v>160</v>
+        <v>273</v>
       </c>
       <c r="F65" s="25" t="str">
-        <f>LEFT(E65, 8)</f>
-        <v>20180814</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G65" s="25">
         <v>0</v>
       </c>
       <c r="H65" s="25">
-        <v>24891</v>
+        <v>24811</v>
       </c>
       <c r="I65" s="25">
-        <v>5526</v>
+        <v>5730</v>
       </c>
       <c r="J65" s="25">
         <v>3000</v>
       </c>
       <c r="K65" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1000</v>
       </c>
       <c r="L65" s="26">
-        <f>I65/D65</f>
-        <v>1842</v>
+        <f t="shared" si="9"/>
+        <v>1910</v>
       </c>
       <c r="M65" s="25">
-        <v>39074</v>
+        <v>39655</v>
       </c>
       <c r="N65" s="25">
         <v>14</v>
       </c>
       <c r="O65" s="25">
-        <v>456</v>
+        <v>472</v>
       </c>
       <c r="P65" s="25">
-        <f>O65/I65</f>
-        <v>8.2519001085776325E-2</v>
+        <f t="shared" si="10"/>
+        <v>8.2373472949389182E-2</v>
       </c>
       <c r="Q65" s="26">
-        <f>O65/D65</f>
-        <v>152</v>
+        <f t="shared" si="11"/>
+        <v>157.33333333333334</v>
       </c>
       <c r="R65" s="25">
-        <v>3226</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" s="25" customFormat="1">
-      <c r="A66" s="25" t="s">
+        <v>3264</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18" s="25" customFormat="1">
+      <c r="B66" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="B66" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C66" s="25" t="s">
         <v>145</v>
@@ -18003,75 +18007,75 @@
         <v>3</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>146</v>
+        <v>274</v>
       </c>
       <c r="F66" s="25" t="str">
-        <f>LEFT(E66, 8)</f>
-        <v>20180815</v>
+        <f t="shared" si="7"/>
+        <v>20180818</v>
       </c>
       <c r="G66" s="25">
         <v>0</v>
       </c>
       <c r="H66" s="25">
-        <v>24643</v>
+        <v>24822</v>
       </c>
       <c r="I66" s="25">
-        <v>6154</v>
+        <v>5980</v>
       </c>
       <c r="J66" s="25">
         <v>3000</v>
       </c>
       <c r="K66" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1000</v>
       </c>
       <c r="L66" s="26">
-        <f>I66/D66</f>
-        <v>2051.3333333333335</v>
+        <f t="shared" si="9"/>
+        <v>1993.3333333333333</v>
       </c>
       <c r="M66" s="25">
-        <v>37504</v>
+        <v>34619</v>
       </c>
       <c r="N66" s="25">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O66" s="25">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="P66" s="25">
-        <f>O66/I66</f>
-        <v>8.4985375365615859E-2</v>
+        <f t="shared" si="10"/>
+        <v>8.8795986622073581E-2</v>
       </c>
       <c r="Q66" s="26">
-        <f>O66/D66</f>
-        <v>174.33333333333334</v>
+        <f t="shared" si="11"/>
+        <v>177</v>
       </c>
       <c r="R66" s="25">
-        <v>3187</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" s="5" customFormat="1">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" s="5" customFormat="1">
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="2:18">
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="2:18">
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="2:18">
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="2:18">
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="2:18">
       <c r="B72" t="s">
         <v>251</v>
       </c>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:18" s="38" customFormat="1">
+    <row r="73" spans="2:18" s="38" customFormat="1">
       <c r="B73" s="38" t="s">
         <v>124</v>
       </c>
@@ -18085,7 +18089,7 @@
         <v>126</v>
       </c>
       <c r="F73" s="38" t="str">
-        <f>LEFT(E73, 8)</f>
+        <f t="shared" ref="F73:F96" si="13">LEFT(E73, 8)</f>
         <v>20180813</v>
       </c>
       <c r="G73" s="38">
@@ -18105,7 +18109,7 @@
         <v>400</v>
       </c>
       <c r="L73" s="39">
-        <f>I73/D73</f>
+        <f t="shared" ref="L73:L96" si="14">I73/D73</f>
         <v>1742</v>
       </c>
       <c r="M73" s="38">
@@ -18118,18 +18122,18 @@
         <v>293</v>
       </c>
       <c r="P73" s="38">
-        <f>O73/I73</f>
+        <f t="shared" ref="P73:P96" si="15">O73/I73</f>
         <v>0.16819747416762343</v>
       </c>
       <c r="Q73" s="39">
-        <f>O73/D73</f>
+        <f t="shared" ref="Q73:Q96" si="16">O73/D73</f>
         <v>293</v>
       </c>
       <c r="R73" s="38">
         <v>270</v>
       </c>
     </row>
-    <row r="74" spans="1:18" s="38" customFormat="1">
+    <row r="74" spans="2:18" s="38" customFormat="1">
       <c r="B74" s="38" t="s">
         <v>124</v>
       </c>
@@ -18143,7 +18147,7 @@
         <v>127</v>
       </c>
       <c r="F74" s="38" t="str">
-        <f>LEFT(E74, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180813</v>
       </c>
       <c r="G74" s="38">
@@ -18159,11 +18163,11 @@
         <v>400</v>
       </c>
       <c r="K74" s="38">
-        <f t="shared" ref="K74:K96" si="8">J74/D74</f>
+        <f t="shared" ref="K74:K96" si="17">J74/D74</f>
         <v>400</v>
       </c>
       <c r="L74" s="39">
-        <f>I74/D74</f>
+        <f t="shared" si="14"/>
         <v>258</v>
       </c>
       <c r="M74" s="38">
@@ -18176,18 +18180,18 @@
         <v>44</v>
       </c>
       <c r="P74" s="38">
-        <f>O74/I74</f>
+        <f t="shared" si="15"/>
         <v>0.17054263565891473</v>
       </c>
       <c r="Q74" s="39">
-        <f>O74/D74</f>
+        <f t="shared" si="16"/>
         <v>44</v>
       </c>
       <c r="R74" s="38">
         <v>162</v>
       </c>
     </row>
-    <row r="75" spans="1:18" s="38" customFormat="1">
+    <row r="75" spans="2:18" s="38" customFormat="1">
       <c r="B75" s="38" t="s">
         <v>124</v>
       </c>
@@ -18201,7 +18205,7 @@
         <v>128</v>
       </c>
       <c r="F75" s="38" t="str">
-        <f>LEFT(E75, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180813</v>
       </c>
       <c r="G75" s="38">
@@ -18217,11 +18221,11 @@
         <v>400</v>
       </c>
       <c r="K75" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>400</v>
       </c>
       <c r="L75" s="39">
-        <f>I75/D75</f>
+        <f t="shared" si="14"/>
         <v>267</v>
       </c>
       <c r="M75" s="38">
@@ -18234,18 +18238,18 @@
         <v>47</v>
       </c>
       <c r="P75" s="38">
-        <f>O75/I75</f>
+        <f t="shared" si="15"/>
         <v>0.17602996254681649</v>
       </c>
       <c r="Q75" s="39">
-        <f>O75/D75</f>
+        <f t="shared" si="16"/>
         <v>47</v>
       </c>
       <c r="R75" s="38">
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="1:18" s="38" customFormat="1">
+    <row r="76" spans="2:18" s="38" customFormat="1">
       <c r="B76" s="38" t="s">
         <v>137</v>
       </c>
@@ -18259,7 +18263,7 @@
         <v>138</v>
       </c>
       <c r="F76" s="38" t="str">
-        <f>LEFT(E76, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G76" s="38">
@@ -18275,11 +18279,11 @@
         <v>400</v>
       </c>
       <c r="K76" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>400</v>
       </c>
       <c r="L76" s="39">
-        <f>I76/D76</f>
+        <f t="shared" si="14"/>
         <v>255</v>
       </c>
       <c r="M76" s="38">
@@ -18292,18 +18296,18 @@
         <v>43</v>
       </c>
       <c r="P76" s="38">
-        <f>O76/I76</f>
+        <f t="shared" si="15"/>
         <v>0.16862745098039217</v>
       </c>
       <c r="Q76" s="39">
-        <f>O76/D76</f>
+        <f t="shared" si="16"/>
         <v>43</v>
       </c>
       <c r="R76" s="38">
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:18" s="38" customFormat="1">
+    <row r="77" spans="2:18" s="38" customFormat="1">
       <c r="B77" s="38" t="s">
         <v>137</v>
       </c>
@@ -18317,7 +18321,7 @@
         <v>139</v>
       </c>
       <c r="F77" s="38" t="str">
-        <f>LEFT(E77, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G77" s="38">
@@ -18333,11 +18337,11 @@
         <v>400</v>
       </c>
       <c r="K77" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>400</v>
       </c>
       <c r="L77" s="39">
-        <f>I77/D77</f>
+        <f t="shared" si="14"/>
         <v>150</v>
       </c>
       <c r="M77" s="38">
@@ -18350,18 +18354,18 @@
         <v>26</v>
       </c>
       <c r="P77" s="38">
-        <f>O77/I77</f>
+        <f t="shared" si="15"/>
         <v>0.17333333333333334</v>
       </c>
       <c r="Q77" s="39">
-        <f>O77/D77</f>
+        <f t="shared" si="16"/>
         <v>26</v>
       </c>
       <c r="R77" s="38">
         <v>170</v>
       </c>
     </row>
-    <row r="78" spans="1:18" s="38" customFormat="1">
+    <row r="78" spans="2:18" s="38" customFormat="1">
       <c r="B78" s="38" t="s">
         <v>137</v>
       </c>
@@ -18375,7 +18379,7 @@
         <v>140</v>
       </c>
       <c r="F78" s="38" t="str">
-        <f>LEFT(E78, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G78" s="38">
@@ -18391,11 +18395,11 @@
         <v>400</v>
       </c>
       <c r="K78" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>400</v>
       </c>
       <c r="L78" s="39">
-        <f>I78/D78</f>
+        <f t="shared" si="14"/>
         <v>242</v>
       </c>
       <c r="M78" s="38">
@@ -18408,18 +18412,18 @@
         <v>44</v>
       </c>
       <c r="P78" s="38">
-        <f>O78/I78</f>
+        <f t="shared" si="15"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="Q78" s="39">
-        <f>O78/D78</f>
+        <f t="shared" si="16"/>
         <v>44</v>
       </c>
       <c r="R78" s="38">
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:18" s="38" customFormat="1">
+    <row r="79" spans="2:18" s="38" customFormat="1">
       <c r="B79" s="38" t="s">
         <v>124</v>
       </c>
@@ -18433,7 +18437,7 @@
         <v>134</v>
       </c>
       <c r="F79" s="38" t="str">
-        <f>LEFT(E79, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180813</v>
       </c>
       <c r="G79" s="38">
@@ -18449,11 +18453,11 @@
         <v>2000</v>
       </c>
       <c r="K79" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>2000</v>
       </c>
       <c r="L79" s="39">
-        <f>I79/D79</f>
+        <f t="shared" si="14"/>
         <v>3904</v>
       </c>
       <c r="M79" s="38">
@@ -18466,18 +18470,18 @@
         <v>339</v>
       </c>
       <c r="P79" s="38">
-        <f>O79/I79</f>
+        <f t="shared" si="15"/>
         <v>8.6834016393442626E-2</v>
       </c>
       <c r="Q79" s="39">
-        <f>O79/D79</f>
+        <f t="shared" si="16"/>
         <v>339</v>
       </c>
       <c r="R79" s="38">
         <v>2074</v>
       </c>
     </row>
-    <row r="80" spans="1:18" s="38" customFormat="1">
+    <row r="80" spans="2:18" s="38" customFormat="1">
       <c r="B80" s="38" t="s">
         <v>124</v>
       </c>
@@ -18491,7 +18495,7 @@
         <v>135</v>
       </c>
       <c r="F80" s="38" t="str">
-        <f>LEFT(E80, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180813</v>
       </c>
       <c r="G80" s="38">
@@ -18507,11 +18511,11 @@
         <v>2000</v>
       </c>
       <c r="K80" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>2000</v>
       </c>
       <c r="L80" s="39">
-        <f>I80/D80</f>
+        <f t="shared" si="14"/>
         <v>3496</v>
       </c>
       <c r="M80" s="38">
@@ -18524,11 +18528,11 @@
         <v>303</v>
       </c>
       <c r="P80" s="38">
-        <f>O80/I80</f>
+        <f t="shared" si="15"/>
         <v>8.6670480549199083E-2</v>
       </c>
       <c r="Q80" s="39">
-        <f>O80/D80</f>
+        <f t="shared" si="16"/>
         <v>303</v>
       </c>
       <c r="R80" s="38">
@@ -18549,7 +18553,7 @@
         <v>136</v>
       </c>
       <c r="F81" s="38" t="str">
-        <f>LEFT(E81, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180813</v>
       </c>
       <c r="G81" s="38">
@@ -18565,11 +18569,11 @@
         <v>2000</v>
       </c>
       <c r="K81" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>2000</v>
       </c>
       <c r="L81" s="39">
-        <f>I81/D81</f>
+        <f t="shared" si="14"/>
         <v>3445</v>
       </c>
       <c r="M81" s="38">
@@ -18582,11 +18586,11 @@
         <v>250</v>
       </c>
       <c r="P81" s="38">
-        <f>O81/I81</f>
+        <f t="shared" si="15"/>
         <v>7.2568940493468792E-2</v>
       </c>
       <c r="Q81" s="39">
-        <f>O81/D81</f>
+        <f t="shared" si="16"/>
         <v>250</v>
       </c>
       <c r="R81" s="38">
@@ -18607,7 +18611,7 @@
         <v>129</v>
       </c>
       <c r="F82" s="38" t="str">
-        <f>LEFT(E82, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180813</v>
       </c>
       <c r="G82" s="38">
@@ -18623,11 +18627,11 @@
         <v>4000</v>
       </c>
       <c r="K82" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>4000</v>
       </c>
       <c r="L82" s="39">
-        <f>I82/D82</f>
+        <f t="shared" si="14"/>
         <v>7585</v>
       </c>
       <c r="M82" s="38">
@@ -18640,11 +18644,11 @@
         <v>661</v>
       </c>
       <c r="P82" s="38">
-        <f>O82/I82</f>
+        <f t="shared" si="15"/>
         <v>8.7145682267633487E-2</v>
       </c>
       <c r="Q82" s="39">
-        <f>O82/D82</f>
+        <f t="shared" si="16"/>
         <v>661</v>
       </c>
       <c r="R82" s="38">
@@ -18665,7 +18669,7 @@
         <v>131</v>
       </c>
       <c r="F83" s="38" t="str">
-        <f>LEFT(E83, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180813</v>
       </c>
       <c r="G83" s="38">
@@ -18681,11 +18685,11 @@
         <v>4000</v>
       </c>
       <c r="K83" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>4000</v>
       </c>
       <c r="L83" s="39">
-        <f>I83/D83</f>
+        <f t="shared" si="14"/>
         <v>7269</v>
       </c>
       <c r="M83" s="38">
@@ -18698,11 +18702,11 @@
         <v>644</v>
       </c>
       <c r="P83" s="38">
-        <f>O83/I83</f>
+        <f t="shared" si="15"/>
         <v>8.8595405145136877E-2</v>
       </c>
       <c r="Q83" s="39">
-        <f>O83/D83</f>
+        <f t="shared" si="16"/>
         <v>644</v>
       </c>
       <c r="R83" s="38">
@@ -18723,7 +18727,7 @@
         <v>132</v>
       </c>
       <c r="F84" s="38" t="str">
-        <f>LEFT(E84, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G84" s="38">
@@ -18739,11 +18743,11 @@
         <v>4000</v>
       </c>
       <c r="K84" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>4000</v>
       </c>
       <c r="L84" s="39">
-        <f>I84/D84</f>
+        <f t="shared" si="14"/>
         <v>7396</v>
       </c>
       <c r="M84" s="38">
@@ -18756,11 +18760,11 @@
         <v>621</v>
       </c>
       <c r="P84" s="38">
-        <f>O84/I84</f>
+        <f t="shared" si="15"/>
         <v>8.3964305029745806E-2</v>
       </c>
       <c r="Q84" s="39">
-        <f>O84/D84</f>
+        <f t="shared" si="16"/>
         <v>621</v>
       </c>
       <c r="R84" s="38">
@@ -18781,7 +18785,7 @@
         <v>148</v>
       </c>
       <c r="F85" s="38" t="str">
-        <f>LEFT(E85, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G85" s="38">
@@ -18797,11 +18801,11 @@
         <v>3000</v>
       </c>
       <c r="K85" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>600</v>
       </c>
       <c r="L85" s="39">
-        <f>I85/D85</f>
+        <f t="shared" si="14"/>
         <v>1172.8</v>
       </c>
       <c r="M85" s="38">
@@ -18814,11 +18818,11 @@
         <v>555</v>
       </c>
       <c r="P85" s="38">
-        <f>O85/I85</f>
+        <f t="shared" si="15"/>
         <v>9.464529331514325E-2</v>
       </c>
       <c r="Q85" s="39">
-        <f>O85/D85</f>
+        <f t="shared" si="16"/>
         <v>111</v>
       </c>
       <c r="R85" s="38">
@@ -18839,7 +18843,7 @@
         <v>149</v>
       </c>
       <c r="F86" s="38" t="str">
-        <f>LEFT(E86, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G86" s="38">
@@ -18855,11 +18859,11 @@
         <v>3000</v>
       </c>
       <c r="K86" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>600</v>
       </c>
       <c r="L86" s="39">
-        <f>I86/D86</f>
+        <f t="shared" si="14"/>
         <v>1227.4000000000001</v>
       </c>
       <c r="M86" s="38">
@@ -18872,11 +18876,11 @@
         <v>562</v>
       </c>
       <c r="P86" s="38">
-        <f>O86/I86</f>
+        <f t="shared" si="15"/>
         <v>9.1575688447124007E-2</v>
       </c>
       <c r="Q86" s="39">
-        <f>O86/D86</f>
+        <f t="shared" si="16"/>
         <v>112.4</v>
       </c>
       <c r="R86" s="38">
@@ -18897,7 +18901,7 @@
         <v>150</v>
       </c>
       <c r="F87" s="38" t="str">
-        <f>LEFT(E87, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180815</v>
       </c>
       <c r="G87" s="38">
@@ -18913,11 +18917,11 @@
         <v>3000</v>
       </c>
       <c r="K87" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>600</v>
       </c>
       <c r="L87" s="39">
-        <f>I87/D87</f>
+        <f t="shared" si="14"/>
         <v>1978.4</v>
       </c>
       <c r="M87" s="38">
@@ -18930,11 +18934,11 @@
         <v>879</v>
       </c>
       <c r="P87" s="38">
-        <f>O87/I87</f>
+        <f t="shared" si="15"/>
         <v>8.8859684593611002E-2</v>
       </c>
       <c r="Q87" s="39">
-        <f>O87/D87</f>
+        <f t="shared" si="16"/>
         <v>175.8</v>
       </c>
       <c r="R87" s="38">
@@ -18955,7 +18959,7 @@
         <v>152</v>
       </c>
       <c r="F88" s="38" t="str">
-        <f>LEFT(E88, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G88" s="38">
@@ -18971,11 +18975,11 @@
         <v>3000</v>
       </c>
       <c r="K88" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>600</v>
       </c>
       <c r="L88" s="39">
-        <f>I88/D88</f>
+        <f t="shared" si="14"/>
         <v>1161.8</v>
       </c>
       <c r="M88" s="38">
@@ -18988,11 +18992,11 @@
         <v>552</v>
       </c>
       <c r="P88" s="38">
-        <f>O88/I88</f>
+        <f t="shared" si="15"/>
         <v>9.5024961266999483E-2</v>
       </c>
       <c r="Q88" s="39">
-        <f>O88/D88</f>
+        <f t="shared" si="16"/>
         <v>110.4</v>
       </c>
       <c r="R88" s="38">
@@ -19013,7 +19017,7 @@
         <v>153</v>
       </c>
       <c r="F89" s="38" t="str">
-        <f>LEFT(E89, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G89" s="38">
@@ -19029,11 +19033,11 @@
         <v>3000</v>
       </c>
       <c r="K89" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>600</v>
       </c>
       <c r="L89" s="39">
-        <f>I89/D89</f>
+        <f t="shared" si="14"/>
         <v>1145</v>
       </c>
       <c r="M89" s="38">
@@ -19046,11 +19050,11 @@
         <v>524</v>
       </c>
       <c r="P89" s="38">
-        <f>O89/I89</f>
+        <f t="shared" si="15"/>
         <v>9.1528384279475988E-2</v>
       </c>
       <c r="Q89" s="39">
-        <f>O89/D89</f>
+        <f t="shared" si="16"/>
         <v>104.8</v>
       </c>
       <c r="R89" s="38">
@@ -19071,7 +19075,7 @@
         <v>154</v>
       </c>
       <c r="F90" s="38" t="str">
-        <f>LEFT(E90, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180815</v>
       </c>
       <c r="G90" s="38">
@@ -19087,11 +19091,11 @@
         <v>3000</v>
       </c>
       <c r="K90" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>600</v>
       </c>
       <c r="L90" s="39">
-        <f>I90/D90</f>
+        <f t="shared" si="14"/>
         <v>1159.2</v>
       </c>
       <c r="M90" s="38">
@@ -19104,11 +19108,11 @@
         <v>532</v>
       </c>
       <c r="P90" s="38">
-        <f>O90/I90</f>
+        <f t="shared" si="15"/>
         <v>9.1787439613526575E-2</v>
       </c>
       <c r="Q90" s="39">
-        <f>O90/D90</f>
+        <f t="shared" si="16"/>
         <v>106.4</v>
       </c>
       <c r="R90" s="38">
@@ -19129,7 +19133,7 @@
         <v>156</v>
       </c>
       <c r="F91" s="38" t="str">
-        <f>LEFT(E91, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G91" s="38">
@@ -19145,11 +19149,11 @@
         <v>3000</v>
       </c>
       <c r="K91" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>600</v>
       </c>
       <c r="L91" s="39">
-        <f>I91/D91</f>
+        <f t="shared" si="14"/>
         <v>1109.5999999999999</v>
       </c>
       <c r="M91" s="38">
@@ -19162,11 +19166,11 @@
         <v>479</v>
       </c>
       <c r="P91" s="38">
-        <f>O91/I91</f>
+        <f t="shared" si="15"/>
         <v>8.6337418889689974E-2</v>
       </c>
       <c r="Q91" s="39">
-        <f>O91/D91</f>
+        <f t="shared" si="16"/>
         <v>95.8</v>
       </c>
       <c r="R91" s="38">
@@ -19187,7 +19191,7 @@
         <v>157</v>
       </c>
       <c r="F92" s="38" t="str">
-        <f>LEFT(E92, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G92" s="38">
@@ -19203,11 +19207,11 @@
         <v>3000</v>
       </c>
       <c r="K92" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>600</v>
       </c>
       <c r="L92" s="39">
-        <f>I92/D92</f>
+        <f t="shared" si="14"/>
         <v>1134.8</v>
       </c>
       <c r="M92" s="38">
@@ -19220,11 +19224,11 @@
         <v>502</v>
       </c>
       <c r="P92" s="38">
-        <f>O92/I92</f>
+        <f t="shared" si="15"/>
         <v>8.8473739866055695E-2</v>
       </c>
       <c r="Q92" s="39">
-        <f>O92/D92</f>
+        <f t="shared" si="16"/>
         <v>100.4</v>
       </c>
       <c r="R92" s="38">
@@ -19245,7 +19249,7 @@
         <v>158</v>
       </c>
       <c r="F93" s="38" t="str">
-        <f>LEFT(E93, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180815</v>
       </c>
       <c r="G93" s="38">
@@ -19261,11 +19265,11 @@
         <v>3000</v>
       </c>
       <c r="K93" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>600</v>
       </c>
       <c r="L93" s="39">
-        <f>I93/D93</f>
+        <f t="shared" si="14"/>
         <v>1381</v>
       </c>
       <c r="M93" s="38">
@@ -19278,11 +19282,11 @@
         <v>597</v>
       </c>
       <c r="P93" s="38">
-        <f>O93/I93</f>
+        <f t="shared" si="15"/>
         <v>8.6459087617668351E-2</v>
       </c>
       <c r="Q93" s="39">
-        <f>O93/D93</f>
+        <f t="shared" si="16"/>
         <v>119.4</v>
       </c>
       <c r="R93" s="38">
@@ -19303,7 +19307,7 @@
         <v>159</v>
       </c>
       <c r="F94" s="38" t="str">
-        <f>LEFT(E94, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G94" s="38">
@@ -19319,11 +19323,11 @@
         <v>3000</v>
       </c>
       <c r="K94" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1000</v>
       </c>
       <c r="L94" s="39">
-        <f>I94/D94</f>
+        <f t="shared" si="14"/>
         <v>1962.6666666666667</v>
       </c>
       <c r="M94" s="38">
@@ -19336,11 +19340,11 @@
         <v>503</v>
       </c>
       <c r="P94" s="38">
-        <f>O94/I94</f>
+        <f t="shared" si="15"/>
         <v>8.5427989130434784E-2</v>
       </c>
       <c r="Q94" s="39">
-        <f>O94/D94</f>
+        <f t="shared" si="16"/>
         <v>167.66666666666666</v>
       </c>
       <c r="R94" s="38">
@@ -19361,7 +19365,7 @@
         <v>160</v>
       </c>
       <c r="F95" s="38" t="str">
-        <f>LEFT(E95, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180814</v>
       </c>
       <c r="G95" s="38">
@@ -19377,11 +19381,11 @@
         <v>3000</v>
       </c>
       <c r="K95" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1000</v>
       </c>
       <c r="L95" s="39">
-        <f>I95/D95</f>
+        <f t="shared" si="14"/>
         <v>1842</v>
       </c>
       <c r="M95" s="38">
@@ -19394,11 +19398,11 @@
         <v>456</v>
       </c>
       <c r="P95" s="38">
-        <f>O95/I95</f>
+        <f t="shared" si="15"/>
         <v>8.2519001085776325E-2</v>
       </c>
       <c r="Q95" s="39">
-        <f>O95/D95</f>
+        <f t="shared" si="16"/>
         <v>152</v>
       </c>
       <c r="R95" s="38">
@@ -19419,7 +19423,7 @@
         <v>146</v>
       </c>
       <c r="F96" s="38" t="str">
-        <f>LEFT(E96, 8)</f>
+        <f t="shared" si="13"/>
         <v>20180815</v>
       </c>
       <c r="G96" s="38">
@@ -19435,11 +19439,11 @@
         <v>3000</v>
       </c>
       <c r="K96" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1000</v>
       </c>
       <c r="L96" s="39">
-        <f>I96/D96</f>
+        <f t="shared" si="14"/>
         <v>2051.3333333333335</v>
       </c>
       <c r="M96" s="38">
@@ -19452,11 +19456,11 @@
         <v>523</v>
       </c>
       <c r="P96" s="38">
-        <f>O96/I96</f>
+        <f t="shared" si="15"/>
         <v>8.4985375365615859E-2</v>
       </c>
       <c r="Q96" s="39">
-        <f>O96/D96</f>
+        <f t="shared" si="16"/>
         <v>174.33333333333334</v>
       </c>
       <c r="R96" s="38">
@@ -19584,9 +19588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD3939F-B255-B24A-99D1-39EFD23212CB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
@@ -38118,7 +38120,7 @@
   <dimension ref="B3:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -38237,7 +38239,7 @@
       </c>
       <c r="C12">
         <f>CORREL(Results!K55:K66,Results!L55:L66)</f>
-        <v>0.78791050738237067</v>
+        <v>0.78895075115954516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>